<commit_message>
[MS-OXWSBTRF]  work item 387788:Upgrade code to E16.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSBTRF/MS-OXWSBTRF_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSBTRF/MS-OXWSBTRF_RequirementSpecification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\InteropO15Dev\TestSuites\O15.1\Exchange\Platinum\ExchangeServerEWSProtocolTestSuites\Exchange Server EWS Protocol Test Suites\Docs\MS-OXWSBTRF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\E16 EWS update\20160310_BTRF\Docs\MS-OXWSBTRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1212,12 +1212,6 @@
     <t>2.2.5.10</t>
   </si>
   <si>
-    <t>[In Prerequisites/Preconditions]The endpoint (4) URL that is returned by either the Autodiscover Publishing Lookup SOAP-Based Web Service Protocol, as described in [MS-OXWSADISC], or the Autodiscover Publishing and Lookup Protocol, as described in [MS-OXDSCLI], is required to form the HTTP request to the Web server that hosts this protocol.</t>
-  </si>
-  <si>
-    <t>[In Prerequisites/Preconditions] The operations that this protocol defines cannot be accessed unless the correct endpoint (4) is identified in the HTTP Web requests that target this protocol.</t>
-  </si>
-  <si>
     <t>[In Messages]In the following sections, the schema definition might differ from the processing rules imposed by the protocol.</t>
   </si>
   <si>
@@ -1402,9 +1396,6 @@
     <t>[In tns:ExportItemsSoapIn Message]This part [request] is required.</t>
   </si>
   <si>
-    <t>[In tns:ExportItemsSoapIn Message]The type of Impersonation is t:ExchangeImpersonation ([MS-OXWSCDATA] section 2.2.5.3).</t>
-  </si>
-  <si>
     <t>[In tns:ExportItemsSoapIn Message] [The part Impersonation] 
 specifies a SOAP header that identifies the user whom the client application is impersonating.</t>
   </si>
@@ -1412,19 +1403,10 @@
     <t>[In tns:ExportItemsSoapIn Message]This part [Impersonation] is optional.</t>
   </si>
   <si>
-    <t>[In tns:ExportItemsSoapIn Message]The type of MailboxCulture is t:MailboxCulture ([MS-OXWSCDATA] section 2.2.5.6).</t>
-  </si>
-  <si>
     <t>[In tns:ExportItemsSoapIn Message] [The part MailboxCulture] specifies a SOAP header that identifies the culture to use for accessing the server. The cultures are defined by [RFC3066].</t>
   </si>
   <si>
-    <t>[In tns:ExportItemsSoapIn Message]The type of RequestVersion is t:RequestServerVersion ([MS-OXWSCDATA] section 2.2.5.9).</t>
-  </si>
-  <si>
     <t>[In tns:ExportItemsSoapIn Message] [RequestVersion] specifies a SOAP header that identifies the schema version for the ExportItems operation request.</t>
-  </si>
-  <si>
-    <t>[In tns:ExportItemsSoapIn Message]The part ManagementRole with Element/type t:ManagementRole ([MS-OXWSCDATA] section 2.2.5.7): specifies the SOAP header that identifies the caller's role. &lt;2&gt; .</t>
   </si>
   <si>
     <t>[In tns:ExportItemsSoapOut Message]The ExportItemsSoapOut WSDL message specifies the SOAP message that represents a response that contains exported items.
@@ -1446,9 +1428,6 @@
     <t>[In tns:ExportItemsSoapOut Message][The part ExportItemsResult] specifies the SOAP body of the response.</t>
   </si>
   <si>
-    <t>[In tns:ExportItemsSoapOut Message]The type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.5.10).</t>
-  </si>
-  <si>
     <t>[In tns:ExportItemsSoapOut Message][The part ServerVersion] specifies the SOAP header that identifies the server version for the response.</t>
   </si>
   <si>
@@ -1459,9 +1438,6 @@
   </si>
   <si>
     <t>[In tns:ExportItemsSoapOut Message]If the request is unsuccessful, the ExportItems operation returns an ExportItemsResponse element with the ResponseClass attribute of the ExportItemsResponseMessage element set to "Error".</t>
-  </si>
-  <si>
-    <t>[In tns:ExportItemsSoapOut Message][If the request is unsuccessful]The ResponseCode element of the ExportItemsResponseMessage element is set to a value of the ResponseCodeType simple type, as specified in [MS-OXWSCDATA] section 2.2.3.23.</t>
   </si>
   <si>
     <t>[In Elements]The following table[in 3.1.4.1.2] lists the XML schema element definitions [ExportItems, ExportItemsResponse] that are specific to this operation[ExportItems].</t>
@@ -1510,9 +1486,6 @@
   </si>
   <si>
     <t>[In m:ExportItemsResponseMessageType Complex Type]The ExportItemsResponseMessageType complex type specifies a single exported item.</t>
-  </si>
-  <si>
-    <t>[In m:ExportItemsResponseMessageType Complex Type]The ExportItemsResponseMessageType complex type extends the ResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.57.</t>
   </si>
   <si>
     <t>[In m:ExportItemsResponseMessageType Complex Type][The schema of ExportItemsResponseMessageType is:]
@@ -1541,9 +1514,6 @@
     <t>[In m:ExportItemsResponseMessageType Complex Type]The following table lists the child elements [ItemId, Data] of the ExportItemsResponseMessageType complex type.</t>
   </si>
   <si>
-    <t>[In m:ExportItemsResponseMessageType Complex Type]The type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.19).</t>
-  </si>
-  <si>
     <t>[In m:ExportItemsResponseMessageType Complex Type][ItemId] specifies the item identifier of a single exported item.</t>
   </si>
   <si>
@@ -1560,9 +1530,6 @@
   </si>
   <si>
     <t>[In ExportItemsResponseType Complex Type]The ExportItemsResponseType complex type specifies a response to export items from a mailbox.</t>
-  </si>
-  <si>
-    <t>[In ExportItemsResponseType Complex Type]The ExportItemsResponseType complex type extends the BaseResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.16.</t>
   </si>
   <si>
     <t>[In ExportItemsResponseType Complex Type][The schema of ExportItemsResponseType is:]
@@ -1576,9 +1543,6 @@
   </si>
   <si>
     <t>[In ExportItemsType Complex Type]The ExportItemsType complex type specifies a request to export items out of a mailbox.</t>
-  </si>
-  <si>
-    <t>[In ExportItemsType Complex Type]The ExportItemsType complex type extends the BaseRequestType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.15.</t>
   </si>
   <si>
     <t>[In ExportItemsType Complex Type][The schema of ExportItemsType is:] &lt;xs:complexType name="ExportItemsType"&gt;
@@ -1613,10 +1577,6 @@
   </si>
   <si>
     <t>[In t:NonEmptyArrayOfItemIdsType Complex Type]The following table lists the child elements[ItemId] of the ExportItemsType complex type.</t>
-  </si>
-  <si>
-    <t>[In t:NonEmptyArrayOfItemIdsType Complex Type]The type of ItemId is 
-t:ItemIdType ([MS-OXWSCORE] section 2.2.4.19).</t>
   </si>
   <si>
     <t>[In t:NonEmptyArrayOfItemIdsType Complex Type][ItemId] specifies the item identifier of an item to export from a mailbox.</t>
@@ -1690,20 +1650,12 @@
     <t>[In tns:UploadItemsSoapIn Message] The request part specifies the SOAP body of the request.</t>
   </si>
   <si>
-    <t>[In tns:UploadItemsSoapIn Message]The Element/type of Impersonation
- is ExchangeImpersonation ([MS-OXWSCDATA] section 2.2.5.3).</t>
-  </si>
-  <si>
     <t>[In tns:UploadItemsSoapIn Message]The Impersonation part specifies a SOAP header that identifies the user whom the client application is impersonating.</t>
   </si>
   <si>
     <t>[In tns:UploadItemsSoapIn Message]This part [Impersonation] is optional.</t>
   </si>
   <si>
-    <t>[In tns:UploadItemsSoapIn Message]The Element/type of MailboxCulture is
-MailboxCulture ([MS-OXWSCDATA] section 2.2.5.6).</t>
-  </si>
-  <si>
     <t>[In tns:UploadItemsSoapIn Message] The MailboxCulture part specifies the SOAP header that identifies the culture to use for accessing the server.</t>
   </si>
   <si>
@@ -1711,10 +1663,6 @@
   </si>
   <si>
     <t>[In tns:UploadItemsSoapIn Message] This part [MailboxCulture] is optional.</t>
-  </si>
-  <si>
-    <t>[In tns:UploadItemsSoapIn Message]The Element/type of RequestVersion is
-RequestServerVersion ([MS-OXWSCDATA] section 2.2.5.9).</t>
   </si>
   <si>
     <t>[In tns:UploadItemsSoapIn Message]The RequestVersion part specifies a SOAP header that identifies the schema version for the UploadItems operation request.</t>
@@ -1740,9 +1688,6 @@
     <t>[In tns:UploadItemsSoapOut Message]The UploadItemsResult part specifies the SOAP body of the response to an UploadItems operation request.</t>
   </si>
   <si>
-    <t>[In tns:UploadItemsSoapOut Message]The Element/type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.5.10).</t>
-  </si>
-  <si>
     <t>[In tns:UploadItemsSoapOut Message]The ServerVersion part specifies the SOAP header that identifies the server version for the response.</t>
   </si>
   <si>
@@ -1753,9 +1698,6 @@
   </si>
   <si>
     <t>[In tns:UploadItemsSoapOut Message]If the request [UploadItems request] is unsuccessful, the UploadItems operation returns an UploadItemsResponse element with the ResponseClass attribute of the UploadItemsResponseMessage element set to "Error".</t>
-  </si>
-  <si>
-    <t>[In tns:UploadItemsSoapOut Message][If the request UploadItems request is unsuccessful]The ResponseCode element of the UploadItemsResponseMessage element is set to a value of the ResponseCodeType simple type, as specified in [MS-OXWSCDATA] section 2.2.3.23.</t>
   </si>
   <si>
     <t>[In Elements]The following table [in 3.1.4.2.2] lists the XML schema element definitions [UploadItems, UploadItemsResponse ] that are specific to this operation[UploadItems].</t>
@@ -1834,9 +1776,6 @@
   </si>
   <si>
     <t>[In m:UploadItemsResponseMessageType Complex Type]The UploadItemsResponseMessageType complex type specifies the item identifier of an item that was uploaded into a mailbox.</t>
-  </si>
-  <si>
-    <t>[In m:UploadItemsResponseMessageType Complex Type]The UploadItemsResponseMessageType complex type extends the ResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.57.</t>
   </si>
   <si>
     <t>[In m:UploadItemsResponseMessageType Complex Type][The schema of UploadItemsResponseMessageType is:]
@@ -1854,9 +1793,6 @@
     <t>[In m:UploadItemsResponseMessageType Complex Type]The following table [in 3.1.4.2.3.2] lists the child elements [ItemId] of the UploadItemsResponseMessageType complex type.</t>
   </si>
   <si>
-    <t>[In m:UploadItemsResponseMessageType Complex Type]The Type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.19).</t>
-  </si>
-  <si>
     <t>[In m:UploadItemsResponseMessageType Complex Type]The ItemId element specifies the item identifier of an item that was uploaded into a mailbox.</t>
   </si>
   <si>
@@ -1864,9 +1800,6 @@
   </si>
   <si>
     <t>[In m:UploadItemsResponseType Complex Type]The UploadItemsResponseType complex type specifies the response messages for which an attempt was made to update into a mailbox.</t>
-  </si>
-  <si>
-    <t>[In m:UploadItemsResponseType Complex Type]The UploadItemsResponseType complex type extends the BaseResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.16.</t>
   </si>
   <si>
     <t>[In m:UploadItemsResponseType Complex Type][The schema of UploadItemsResponseType is:]
@@ -1878,9 +1811,6 @@
   </si>
   <si>
     <t>[In m:UploadItemsType Complex Type]The UploadItemsType complex type specifies the contents of a request to upload items in to a mailbox.</t>
-  </si>
-  <si>
-    <t>[In m:UploadItemsType Complex Type]The UploadItemsType complex type extends the BaseRequestType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.15.</t>
   </si>
   <si>
     <t>[In m:UploadItemsType Complex Type][The schema of UploadItemsType is:]
@@ -1922,16 +1852,10 @@
     <t>[In m:UploadItemType Complex Type]The following table [in 3.1.4.2.3.5] lists the child elements [ParentFolderId, ItemId, Data] of the UploadItemType complex type.</t>
   </si>
   <si>
-    <t>[In m:UploadItemType Complex Type]The Type of ParentFolderId is t:FolderIdType ([MS-OXWSCDATA] section 2.2.4.31).</t>
-  </si>
-  <si>
     <t>[In m:UploadItemType Complex Type][ParentFolderId] specifies the target folder in which to place the upload item.</t>
   </si>
   <si>
     <t>[In m:UploadItemType Complex Type] This element [ParentFolderId] MUST be present.</t>
-  </si>
-  <si>
-    <t>[In m:UploadItemType Complex Type]The Type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.19).</t>
   </si>
   <si>
     <t>[In m:UploadItemType Complex Type][ItemId] specifies the item identifier of the upload item.</t>
@@ -2838,6 +2762,106 @@
   </si>
   <si>
     <t>This column explains the reason why the requirement is non-testable or unverified (for Normative, InScope requirements).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Prerequisites/Preconditions]The endpoint URL that is returned by either the Autodiscover Publishing Lookup SOAP-Based Web Service Protocol, as described in [MS-OXWSADISC], or the Autodiscover Publishing and Lookup Protocol, as described in [MS-OXDSCLI], is required to form the HTTP request to the Web server that hosts this protocol.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Prerequisites/Preconditions] The operations that this protocol defines cannot be accessed unless the correct endpoint is identified in the HTTP Web requests that target this protocol.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapIn Message]The type of Impersonation is t:ExchangeImpersonation ([MS-OXWSCDATA] section 2.2.3.3).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapIn Message]The type of MailboxCulture is t:MailboxCulture ([MS-OXWSCDATA] section 2.2.3.7).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapIn Message]The type of RequestVersion is t:RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.11).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapIn Message]The part ManagementRole with Element/type t:ManagementRole ([MS-OXWSCDATA] section 2.2.3.8): specifies the SOAP header that identifies the caller's role. &lt;2&gt; .</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapOut Message]The type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.3.12).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapOut Message][If the request is unsuccessful]The ResponseCode element of the ExportItemsResponseMessage element is set to a value of the ResponseCodeType simple type, as specified in [MS-OXWSCDATA] section 2.2.5.24.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:ExportItemsResponseMessageType Complex Type]The ExportItemsResponseMessageType complex type extends the ResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.67.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:ExportItemsResponseMessageType Complex Type]The type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In ExportItemsResponseType Complex Type]The ExportItemsResponseType complex type extends the BaseResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.18.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In ExportItemsType Complex Type]The ExportItemsType complex type extends the BaseRequestType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.17.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:NonEmptyArrayOfItemIdsType Complex Type]The type of ItemId is 
+t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:UploadItemsSoapIn Message]The Element/type of Impersonation
+ is ExchangeImpersonation ([MS-OXWSCDATA] section 2.2.3.3).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:UploadItemsSoapIn Message]The Element/type of MailboxCulture is
+MailboxCulture ([MS-OXWSCDATA] section 2.2.3.7).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:UploadItemsSoapIn Message]The Element/type of RequestVersion is
+RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.11).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:UploadItemsSoapOut Message][If the request UploadItems request is unsuccessful]The ResponseCode element of the UploadItemsResponseMessage element is set to a value of the ResponseCodeType simple type, as specified in [MS-OXWSCDATA] section 2.2.5.24.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:UploadItemsSoapOut Message]The Element/type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.3.12).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:UploadItemsResponseMessageType Complex Type]The UploadItemsResponseMessageType complex type extends the ResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.67.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:UploadItemsResponseMessageType Complex Type]The Type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:UploadItemsResponseType Complex Type]The UploadItemsResponseType complex type extends the BaseResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.18.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:UploadItemsType Complex Type]The UploadItemsType complex type extends the BaseRequestType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.17.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:UploadItemType Complex Type]The Type of ParentFolderId is t:FolderIdType ([MS-OXWSCDATA] section 2.2.4.36).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:UploadItemType Complex Type]The Type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4166,7 +4190,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>558</v>
+        <v>534</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -4178,7 +4202,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>559</v>
+        <v>535</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4196,14 +4220,14 @@
         <v>25</v>
       </c>
       <c r="C3" s="36">
-        <v>4.0999999999999996</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="35" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="37">
-        <v>41185</v>
+        <v>42261</v>
       </c>
       <c r="G3" s="38"/>
       <c r="H3" s="4"/>
@@ -4282,7 +4306,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>563</v>
+        <v>539</v>
       </c>
       <c r="C8" s="55"/>
       <c r="D8" s="55"/>
@@ -4333,7 +4357,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>564</v>
+        <v>540</v>
       </c>
       <c r="C11" s="61"/>
       <c r="D11" s="47"/>
@@ -4460,7 +4484,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>565</v>
+        <v>541</v>
       </c>
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
@@ -4511,7 +4535,7 @@
         <v>274</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>321</v>
+        <v>542</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18" t="s">
@@ -4536,7 +4560,7 @@
         <v>274</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>322</v>
+        <v>543</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18" t="s">
@@ -4561,7 +4585,7 @@
         <v>275</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18" t="s">
@@ -4586,7 +4610,7 @@
         <v>275</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18" t="s">
@@ -4611,7 +4635,7 @@
         <v>275</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18" t="s">
@@ -4636,7 +4660,7 @@
         <v>275</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18" t="s">
@@ -4661,7 +4685,7 @@
         <v>275</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18" t="s">
@@ -4686,7 +4710,7 @@
         <v>276</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18" t="s">
@@ -4711,7 +4735,7 @@
         <v>276</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="18" t="s">
@@ -4736,7 +4760,7 @@
         <v>276</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18" t="s">
@@ -4753,7 +4777,7 @@
       </c>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:13" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="s">
         <v>50</v>
       </c>
@@ -4761,7 +4785,7 @@
         <v>276</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18" t="s">
@@ -4777,7 +4801,7 @@
         <v>17</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>556</v>
+        <v>532</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4788,7 +4812,7 @@
         <v>277</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18" t="s">
@@ -4813,7 +4837,7 @@
         <v>277</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18" t="s">
@@ -4838,7 +4862,7 @@
         <v>278</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18" t="s">
@@ -4863,7 +4887,7 @@
         <v>278</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="25" t="s">
@@ -4888,7 +4912,7 @@
         <v>278</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="25" t="s">
@@ -4913,7 +4937,7 @@
         <v>278</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="25" t="s">
@@ -4938,7 +4962,7 @@
         <v>278</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="25" t="s">
@@ -4963,7 +4987,7 @@
         <v>278</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="25" t="s">
@@ -4988,7 +5012,7 @@
         <v>278</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="25" t="s">
@@ -5013,7 +5037,7 @@
         <v>278</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="25" t="s">
@@ -5038,7 +5062,7 @@
         <v>278</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D41" s="25"/>
       <c r="E41" s="25" t="s">
@@ -5063,7 +5087,7 @@
         <v>278</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D42" s="25"/>
       <c r="E42" s="25" t="s">
@@ -5088,7 +5112,7 @@
         <v>279</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D43" s="25"/>
       <c r="E43" s="25" t="s">
@@ -5113,7 +5137,7 @@
         <v>280</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="25" t="s">
@@ -5138,7 +5162,7 @@
         <v>281</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D45" s="25"/>
       <c r="E45" s="25" t="s">
@@ -5163,7 +5187,7 @@
         <v>282</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D46" s="25"/>
       <c r="E46" s="25" t="s">
@@ -5188,7 +5212,7 @@
         <v>283</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="25" t="s">
@@ -5213,7 +5237,7 @@
         <v>284</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D48" s="25"/>
       <c r="E48" s="25" t="s">
@@ -5238,7 +5262,7 @@
         <v>285</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="25" t="s">
@@ -5263,7 +5287,7 @@
         <v>286</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D50" s="25"/>
       <c r="E50" s="25" t="s">
@@ -5288,7 +5312,7 @@
         <v>286</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="25" t="s">
@@ -5313,7 +5337,7 @@
         <v>286</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D52" s="25"/>
       <c r="E52" s="25" t="s">
@@ -5338,7 +5362,7 @@
         <v>287</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D53" s="25"/>
       <c r="E53" s="25" t="s">
@@ -5363,7 +5387,7 @@
         <v>287</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="25" t="s">
@@ -5388,7 +5412,7 @@
         <v>288</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D55" s="25"/>
       <c r="E55" s="25" t="s">
@@ -5413,7 +5437,7 @@
         <v>288</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D56" s="25"/>
       <c r="E56" s="25" t="s">
@@ -5438,7 +5462,7 @@
         <v>288</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D57" s="25"/>
       <c r="E57" s="25" t="s">
@@ -5463,7 +5487,7 @@
         <v>288</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D58" s="25"/>
       <c r="E58" s="25" t="s">
@@ -5488,7 +5512,7 @@
         <v>31</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D59" s="25"/>
       <c r="E59" s="25" t="s">
@@ -5513,7 +5537,7 @@
         <v>31</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D60" s="25"/>
       <c r="E60" s="25" t="s">
@@ -5538,7 +5562,7 @@
         <v>31</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D61" s="25"/>
       <c r="E61" s="25" t="s">
@@ -5554,7 +5578,7 @@
         <v>17</v>
       </c>
       <c r="I61" s="27" t="s">
-        <v>560</v>
+        <v>536</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5565,7 +5589,7 @@
         <v>289</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D62" s="25"/>
       <c r="E62" s="25" t="s">
@@ -5590,7 +5614,7 @@
         <v>289</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D63" s="25"/>
       <c r="E63" s="25" t="s">
@@ -5615,7 +5639,7 @@
         <v>289</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D64" s="25"/>
       <c r="E64" s="25" t="s">
@@ -5640,7 +5664,7 @@
         <v>290</v>
       </c>
       <c r="C65" s="27" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D65" s="25"/>
       <c r="E65" s="25" t="s">
@@ -5665,7 +5689,7 @@
         <v>290</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D66" s="25"/>
       <c r="E66" s="25" t="s">
@@ -5690,7 +5714,7 @@
         <v>290</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D67" s="25"/>
       <c r="E67" s="25" t="s">
@@ -5715,7 +5739,7 @@
         <v>290</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25" t="s">
@@ -5740,7 +5764,7 @@
         <v>290</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D69" s="25"/>
       <c r="E69" s="25" t="s">
@@ -5765,7 +5789,7 @@
         <v>290</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D70" s="25"/>
       <c r="E70" s="25" t="s">
@@ -5790,7 +5814,7 @@
         <v>290</v>
       </c>
       <c r="C71" s="27" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D71" s="25"/>
       <c r="E71" s="25" t="s">
@@ -5814,8 +5838,8 @@
       <c r="B72" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="C72" s="27" t="s">
-        <v>373</v>
+      <c r="C72" s="16" t="s">
+        <v>544</v>
       </c>
       <c r="D72" s="25"/>
       <c r="E72" s="25" t="s">
@@ -5840,7 +5864,7 @@
         <v>290</v>
       </c>
       <c r="C73" s="27" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D73" s="25"/>
       <c r="E73" s="25" t="s">
@@ -5865,7 +5889,7 @@
         <v>290</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D74" s="25"/>
       <c r="E74" s="25" t="s">
@@ -5889,8 +5913,8 @@
       <c r="B75" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="C75" s="27" t="s">
-        <v>376</v>
+      <c r="C75" s="16" t="s">
+        <v>545</v>
       </c>
       <c r="D75" s="25"/>
       <c r="E75" s="25" t="s">
@@ -5915,7 +5939,7 @@
         <v>290</v>
       </c>
       <c r="C76" s="27" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D76" s="25"/>
       <c r="E76" s="25" t="s">
@@ -5939,8 +5963,8 @@
       <c r="B77" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="C77" s="27" t="s">
-        <v>378</v>
+      <c r="C77" s="16" t="s">
+        <v>546</v>
       </c>
       <c r="D77" s="25"/>
       <c r="E77" s="25" t="s">
@@ -5965,7 +5989,7 @@
         <v>290</v>
       </c>
       <c r="C78" s="27" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D78" s="25"/>
       <c r="E78" s="25" t="s">
@@ -5989,8 +6013,8 @@
       <c r="B79" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="C79" s="27" t="s">
-        <v>380</v>
+      <c r="C79" s="16" t="s">
+        <v>547</v>
       </c>
       <c r="D79" s="25"/>
       <c r="E79" s="25" t="s">
@@ -6015,7 +6039,7 @@
         <v>291</v>
       </c>
       <c r="C80" s="27" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D80" s="25"/>
       <c r="E80" s="25" t="s">
@@ -6040,7 +6064,7 @@
         <v>291</v>
       </c>
       <c r="C81" s="27" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="D81" s="25"/>
       <c r="E81" s="25" t="s">
@@ -6065,7 +6089,7 @@
         <v>291</v>
       </c>
       <c r="C82" s="27" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D82" s="25"/>
       <c r="E82" s="25" t="s">
@@ -6090,7 +6114,7 @@
         <v>291</v>
       </c>
       <c r="C83" s="27" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="D83" s="25"/>
       <c r="E83" s="25" t="s">
@@ -6115,7 +6139,7 @@
         <v>291</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D84" s="25"/>
       <c r="E84" s="25" t="s">
@@ -6139,8 +6163,8 @@
       <c r="B85" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="C85" s="27" t="s">
-        <v>386</v>
+      <c r="C85" s="16" t="s">
+        <v>548</v>
       </c>
       <c r="D85" s="25"/>
       <c r="E85" s="25" t="s">
@@ -6165,7 +6189,7 @@
         <v>291</v>
       </c>
       <c r="C86" s="27" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="D86" s="25"/>
       <c r="E86" s="25" t="s">
@@ -6190,7 +6214,7 @@
         <v>291</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="D87" s="25"/>
       <c r="E87" s="25" t="s">
@@ -6215,7 +6239,7 @@
         <v>291</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="D88" s="25"/>
       <c r="E88" s="25" t="s">
@@ -6240,7 +6264,7 @@
         <v>291</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="D89" s="25"/>
       <c r="E89" s="25" t="s">
@@ -6264,8 +6288,8 @@
       <c r="B90" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="C90" s="27" t="s">
-        <v>391</v>
+      <c r="C90" s="16" t="s">
+        <v>549</v>
       </c>
       <c r="D90" s="25"/>
       <c r="E90" s="25" t="s">
@@ -6290,7 +6314,7 @@
         <v>292</v>
       </c>
       <c r="C91" s="27" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="D91" s="25"/>
       <c r="E91" s="25" t="s">
@@ -6315,7 +6339,7 @@
         <v>292</v>
       </c>
       <c r="C92" s="27" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D92" s="25"/>
       <c r="E92" s="25" t="s">
@@ -6340,7 +6364,7 @@
         <v>292</v>
       </c>
       <c r="C93" s="27" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="D93" s="25"/>
       <c r="E93" s="25" t="s">
@@ -6365,7 +6389,7 @@
         <v>293</v>
       </c>
       <c r="C94" s="27" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="D94" s="25"/>
       <c r="E94" s="25" t="s">
@@ -6390,7 +6414,7 @@
         <v>293</v>
       </c>
       <c r="C95" s="27" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="D95" s="25"/>
       <c r="E95" s="25" t="s">
@@ -6415,7 +6439,7 @@
         <v>293</v>
       </c>
       <c r="C96" s="27" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="D96" s="25"/>
       <c r="E96" s="25" t="s">
@@ -6440,7 +6464,7 @@
         <v>294</v>
       </c>
       <c r="C97" s="27" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="D97" s="25"/>
       <c r="E97" s="25" t="s">
@@ -6465,7 +6489,7 @@
         <v>294</v>
       </c>
       <c r="C98" s="27" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D98" s="25"/>
       <c r="E98" s="25" t="s">
@@ -6490,7 +6514,7 @@
         <v>294</v>
       </c>
       <c r="C99" s="27" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="D99" s="25"/>
       <c r="E99" s="25" t="s">
@@ -6515,7 +6539,7 @@
         <v>295</v>
       </c>
       <c r="C100" s="27" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="D100" s="25"/>
       <c r="E100" s="25" t="s">
@@ -6540,7 +6564,7 @@
         <v>295</v>
       </c>
       <c r="C101" s="27" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="D101" s="25"/>
       <c r="E101" s="25" t="s">
@@ -6565,7 +6589,7 @@
         <v>295</v>
       </c>
       <c r="C102" s="27" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="D102" s="25"/>
       <c r="E102" s="25" t="s">
@@ -6590,7 +6614,7 @@
         <v>295</v>
       </c>
       <c r="C103" s="27" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="D103" s="25"/>
       <c r="E103" s="25" t="s">
@@ -6615,7 +6639,7 @@
         <v>295</v>
       </c>
       <c r="C104" s="27" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D104" s="25"/>
       <c r="E104" s="25" t="s">
@@ -6640,7 +6664,7 @@
         <v>296</v>
       </c>
       <c r="C105" s="27" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="D105" s="25"/>
       <c r="E105" s="25" t="s">
@@ -6664,8 +6688,8 @@
       <c r="B106" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="C106" s="27" t="s">
-        <v>407</v>
+      <c r="C106" s="16" t="s">
+        <v>550</v>
       </c>
       <c r="D106" s="25"/>
       <c r="E106" s="25" t="s">
@@ -6690,7 +6714,7 @@
         <v>296</v>
       </c>
       <c r="C107" s="27" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="D107" s="25"/>
       <c r="E107" s="25" t="s">
@@ -6715,7 +6739,7 @@
         <v>296</v>
       </c>
       <c r="C108" s="27" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="D108" s="25"/>
       <c r="E108" s="25" t="s">
@@ -6739,8 +6763,8 @@
       <c r="B109" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="C109" s="27" t="s">
-        <v>410</v>
+      <c r="C109" s="16" t="s">
+        <v>551</v>
       </c>
       <c r="D109" s="25"/>
       <c r="E109" s="25" t="s">
@@ -6765,7 +6789,7 @@
         <v>296</v>
       </c>
       <c r="C110" s="27" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="D110" s="25"/>
       <c r="E110" s="25" t="s">
@@ -6790,7 +6814,7 @@
         <v>296</v>
       </c>
       <c r="C111" s="27" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="D111" s="25"/>
       <c r="E111" s="25" t="s">
@@ -6815,7 +6839,7 @@
         <v>296</v>
       </c>
       <c r="C112" s="27" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="D112" s="25"/>
       <c r="E112" s="25" t="s">
@@ -6840,7 +6864,7 @@
         <v>296</v>
       </c>
       <c r="C113" s="27" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="D113" s="25"/>
       <c r="E113" s="25" t="s">
@@ -6865,7 +6889,7 @@
         <v>296</v>
       </c>
       <c r="C114" s="27" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="D114" s="25"/>
       <c r="E114" s="25" t="s">
@@ -6890,7 +6914,7 @@
         <v>297</v>
       </c>
       <c r="C115" s="27" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="D115" s="25"/>
       <c r="E115" s="25" t="s">
@@ -6914,8 +6938,8 @@
       <c r="B116" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="C116" s="27" t="s">
-        <v>417</v>
+      <c r="C116" s="16" t="s">
+        <v>552</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="25" t="s">
@@ -6940,7 +6964,7 @@
         <v>297</v>
       </c>
       <c r="C117" s="27" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="25" t="s">
@@ -6965,7 +6989,7 @@
         <v>298</v>
       </c>
       <c r="C118" s="27" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="25" t="s">
@@ -6989,8 +7013,8 @@
       <c r="B119" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="C119" s="27" t="s">
-        <v>420</v>
+      <c r="C119" s="16" t="s">
+        <v>553</v>
       </c>
       <c r="D119" s="25"/>
       <c r="E119" s="25" t="s">
@@ -7015,7 +7039,7 @@
         <v>298</v>
       </c>
       <c r="C120" s="27" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="D120" s="25"/>
       <c r="E120" s="25" t="s">
@@ -7040,7 +7064,7 @@
         <v>298</v>
       </c>
       <c r="C121" s="27" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="25" t="s">
@@ -7065,7 +7089,7 @@
         <v>298</v>
       </c>
       <c r="C122" s="27" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="D122" s="25"/>
       <c r="E122" s="25" t="s">
@@ -7090,7 +7114,7 @@
         <v>298</v>
       </c>
       <c r="C123" s="27" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="D123" s="25"/>
       <c r="E123" s="25" t="s">
@@ -7115,7 +7139,7 @@
         <v>298</v>
       </c>
       <c r="C124" s="27" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="D124" s="25"/>
       <c r="E124" s="25" t="s">
@@ -7140,7 +7164,7 @@
         <v>299</v>
       </c>
       <c r="C125" s="27" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D125" s="25"/>
       <c r="E125" s="25" t="s">
@@ -7165,7 +7189,7 @@
         <v>299</v>
       </c>
       <c r="C126" s="27" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="D126" s="25"/>
       <c r="E126" s="25" t="s">
@@ -7189,8 +7213,8 @@
       <c r="B127" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="C127" s="27" t="s">
-        <v>428</v>
+      <c r="C127" s="16" t="s">
+        <v>554</v>
       </c>
       <c r="D127" s="25"/>
       <c r="E127" s="25" t="s">
@@ -7215,7 +7239,7 @@
         <v>299</v>
       </c>
       <c r="C128" s="27" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="D128" s="25"/>
       <c r="E128" s="25" t="s">
@@ -7240,7 +7264,7 @@
         <v>299</v>
       </c>
       <c r="C129" s="27" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="25" t="s">
@@ -7265,7 +7289,7 @@
         <v>299</v>
       </c>
       <c r="C130" s="27" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="D130" s="25"/>
       <c r="E130" s="25" t="s">
@@ -7290,7 +7314,7 @@
         <v>32</v>
       </c>
       <c r="C131" s="27" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="D131" s="25"/>
       <c r="E131" s="25" t="s">
@@ -7315,7 +7339,7 @@
         <v>32</v>
       </c>
       <c r="C132" s="27" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="D132" s="25"/>
       <c r="E132" s="25" t="s">
@@ -7340,7 +7364,7 @@
         <v>32</v>
       </c>
       <c r="C133" s="27" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="D133" s="25"/>
       <c r="E133" s="25" t="s">
@@ -7365,7 +7389,7 @@
         <v>300</v>
       </c>
       <c r="C134" s="27" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="D134" s="25"/>
       <c r="E134" s="25" t="s">
@@ -7390,7 +7414,7 @@
         <v>300</v>
       </c>
       <c r="C135" s="27" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="D135" s="25"/>
       <c r="E135" s="25" t="s">
@@ -7415,7 +7439,7 @@
         <v>300</v>
       </c>
       <c r="C136" s="27" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="D136" s="25"/>
       <c r="E136" s="25" t="s">
@@ -7440,7 +7464,7 @@
         <v>301</v>
       </c>
       <c r="C137" s="27" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="D137" s="25"/>
       <c r="E137" s="25" t="s">
@@ -7465,7 +7489,7 @@
         <v>301</v>
       </c>
       <c r="C138" s="27" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="D138" s="25"/>
       <c r="E138" s="25" t="s">
@@ -7490,7 +7514,7 @@
         <v>301</v>
       </c>
       <c r="C139" s="27" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="D139" s="25"/>
       <c r="E139" s="25" t="s">
@@ -7515,7 +7539,7 @@
         <v>301</v>
       </c>
       <c r="C140" s="27" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="D140" s="25"/>
       <c r="E140" s="25" t="s">
@@ -7540,7 +7564,7 @@
         <v>301</v>
       </c>
       <c r="C141" s="27" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="D141" s="25"/>
       <c r="E141" s="25" t="s">
@@ -7565,7 +7589,7 @@
         <v>301</v>
       </c>
       <c r="C142" s="27" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="D142" s="25"/>
       <c r="E142" s="25" t="s">
@@ -7589,8 +7613,8 @@
       <c r="B143" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="C143" s="27" t="s">
-        <v>444</v>
+      <c r="C143" s="16" t="s">
+        <v>555</v>
       </c>
       <c r="D143" s="25"/>
       <c r="E143" s="25" t="s">
@@ -7615,7 +7639,7 @@
         <v>301</v>
       </c>
       <c r="C144" s="27" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="D144" s="25"/>
       <c r="E144" s="25" t="s">
@@ -7640,7 +7664,7 @@
         <v>301</v>
       </c>
       <c r="C145" s="27" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="25" t="s">
@@ -7664,8 +7688,8 @@
       <c r="B146" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="C146" s="27" t="s">
-        <v>447</v>
+      <c r="C146" s="16" t="s">
+        <v>556</v>
       </c>
       <c r="D146" s="25"/>
       <c r="E146" s="25" t="s">
@@ -7690,7 +7714,7 @@
         <v>301</v>
       </c>
       <c r="C147" s="27" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="D147" s="25"/>
       <c r="E147" s="25" t="s">
@@ -7715,7 +7739,7 @@
         <v>301</v>
       </c>
       <c r="C148" s="27" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="D148" s="25"/>
       <c r="E148" s="25" t="s">
@@ -7740,7 +7764,7 @@
         <v>301</v>
       </c>
       <c r="C149" s="27" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="25" t="s">
@@ -7764,8 +7788,8 @@
       <c r="B150" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="C150" s="27" t="s">
-        <v>451</v>
+      <c r="C150" s="16" t="s">
+        <v>557</v>
       </c>
       <c r="D150" s="25"/>
       <c r="E150" s="25" t="s">
@@ -7790,7 +7814,7 @@
         <v>301</v>
       </c>
       <c r="C151" s="27" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
       <c r="D151" s="25"/>
       <c r="E151" s="25" t="s">
@@ -7815,7 +7839,7 @@
         <v>302</v>
       </c>
       <c r="C152" s="27" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
       <c r="D152" s="25"/>
       <c r="E152" s="25" t="s">
@@ -7840,7 +7864,7 @@
         <v>302</v>
       </c>
       <c r="C153" s="27" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
       <c r="D153" s="25"/>
       <c r="E153" s="25" t="s">
@@ -7865,7 +7889,7 @@
         <v>302</v>
       </c>
       <c r="C154" s="27" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
       <c r="D154" s="25"/>
       <c r="E154" s="25" t="s">
@@ -7890,7 +7914,7 @@
         <v>302</v>
       </c>
       <c r="C155" s="27" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="D155" s="25"/>
       <c r="E155" s="25" t="s">
@@ -7915,7 +7939,7 @@
         <v>302</v>
       </c>
       <c r="C156" s="27" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="D156" s="25"/>
       <c r="E156" s="25" t="s">
@@ -7939,8 +7963,8 @@
       <c r="B157" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="C157" s="27" t="s">
-        <v>458</v>
+      <c r="C157" s="16" t="s">
+        <v>559</v>
       </c>
       <c r="D157" s="25"/>
       <c r="E157" s="25" t="s">
@@ -7965,7 +7989,7 @@
         <v>302</v>
       </c>
       <c r="C158" s="27" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="D158" s="25"/>
       <c r="E158" s="25" t="s">
@@ -7990,7 +8014,7 @@
         <v>302</v>
       </c>
       <c r="C159" s="27" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
       <c r="D159" s="25"/>
       <c r="E159" s="25" t="s">
@@ -8015,7 +8039,7 @@
         <v>302</v>
       </c>
       <c r="C160" s="27" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="D160" s="25"/>
       <c r="E160" s="25" t="s">
@@ -8040,7 +8064,7 @@
         <v>302</v>
       </c>
       <c r="C161" s="27" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="D161" s="25"/>
       <c r="E161" s="25" t="s">
@@ -8064,8 +8088,8 @@
       <c r="B162" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="C162" s="27" t="s">
-        <v>463</v>
+      <c r="C162" s="16" t="s">
+        <v>558</v>
       </c>
       <c r="D162" s="25"/>
       <c r="E162" s="25" t="s">
@@ -8090,7 +8114,7 @@
         <v>303</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c r="D163" s="25"/>
       <c r="E163" s="25" t="s">
@@ -8115,7 +8139,7 @@
         <v>303</v>
       </c>
       <c r="C164" s="27" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="D164" s="25"/>
       <c r="E164" s="25" t="s">
@@ -8140,7 +8164,7 @@
         <v>303</v>
       </c>
       <c r="C165" s="27" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="D165" s="25"/>
       <c r="E165" s="25" t="s">
@@ -8165,7 +8189,7 @@
         <v>303</v>
       </c>
       <c r="C166" s="27" t="s">
-        <v>467</v>
+        <v>449</v>
       </c>
       <c r="D166" s="25"/>
       <c r="E166" s="25" t="s">
@@ -8190,7 +8214,7 @@
         <v>303</v>
       </c>
       <c r="C167" s="27" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="D167" s="25"/>
       <c r="E167" s="25" t="s">
@@ -8215,7 +8239,7 @@
         <v>304</v>
       </c>
       <c r="C168" s="27" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="D168" s="25"/>
       <c r="E168" s="25" t="s">
@@ -8240,7 +8264,7 @@
         <v>304</v>
       </c>
       <c r="C169" s="27" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="D169" s="25"/>
       <c r="E169" s="25" t="s">
@@ -8265,7 +8289,7 @@
         <v>304</v>
       </c>
       <c r="C170" s="27" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="D170" s="25"/>
       <c r="E170" s="25" t="s">
@@ -8290,7 +8314,7 @@
         <v>305</v>
       </c>
       <c r="C171" s="27" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="D171" s="25"/>
       <c r="E171" s="25" t="s">
@@ -8315,7 +8339,7 @@
         <v>305</v>
       </c>
       <c r="C172" s="27" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="D172" s="25"/>
       <c r="E172" s="25" t="s">
@@ -8340,7 +8364,7 @@
         <v>305</v>
       </c>
       <c r="C173" s="27" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="D173" s="25"/>
       <c r="E173" s="25" t="s">
@@ -8365,7 +8389,7 @@
         <v>306</v>
       </c>
       <c r="C174" s="27" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="D174" s="25"/>
       <c r="E174" s="25" t="s">
@@ -8390,7 +8414,7 @@
         <v>306</v>
       </c>
       <c r="C175" s="27" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="D175" s="25"/>
       <c r="E175" s="25" t="s">
@@ -8415,7 +8439,7 @@
         <v>306</v>
       </c>
       <c r="C176" s="27" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="D176" s="25"/>
       <c r="E176" s="25" t="s">
@@ -8440,7 +8464,7 @@
         <v>306</v>
       </c>
       <c r="C177" s="27" t="s">
-        <v>478</v>
+        <v>460</v>
       </c>
       <c r="D177" s="25"/>
       <c r="E177" s="25" t="s">
@@ -8465,7 +8489,7 @@
         <v>306</v>
       </c>
       <c r="C178" s="27" t="s">
-        <v>479</v>
+        <v>461</v>
       </c>
       <c r="D178" s="25"/>
       <c r="E178" s="25" t="s">
@@ -8490,7 +8514,7 @@
         <v>306</v>
       </c>
       <c r="C179" s="27" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
       <c r="D179" s="25"/>
       <c r="E179" s="25" t="s">
@@ -8515,7 +8539,7 @@
         <v>307</v>
       </c>
       <c r="C180" s="27" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="D180" s="25"/>
       <c r="E180" s="25" t="s">
@@ -8540,7 +8564,7 @@
         <v>307</v>
       </c>
       <c r="C181" s="27" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="D181" s="25"/>
       <c r="E181" s="25" t="s">
@@ -8565,7 +8589,7 @@
         <v>307</v>
       </c>
       <c r="C182" s="27" t="s">
-        <v>483</v>
+        <v>465</v>
       </c>
       <c r="D182" s="25"/>
       <c r="E182" s="25" t="s">
@@ -8590,7 +8614,7 @@
         <v>307</v>
       </c>
       <c r="C183" s="27" t="s">
-        <v>484</v>
+        <v>466</v>
       </c>
       <c r="D183" s="25"/>
       <c r="E183" s="25" t="s">
@@ -8615,7 +8639,7 @@
         <v>307</v>
       </c>
       <c r="C184" s="27" t="s">
-        <v>485</v>
+        <v>467</v>
       </c>
       <c r="D184" s="25"/>
       <c r="E184" s="25" t="s">
@@ -8640,7 +8664,7 @@
         <v>308</v>
       </c>
       <c r="C185" s="27" t="s">
-        <v>486</v>
+        <v>468</v>
       </c>
       <c r="D185" s="25"/>
       <c r="E185" s="25" t="s">
@@ -8664,8 +8688,8 @@
       <c r="B186" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="C186" s="27" t="s">
-        <v>487</v>
+      <c r="C186" s="16" t="s">
+        <v>560</v>
       </c>
       <c r="D186" s="25"/>
       <c r="E186" s="25" t="s">
@@ -8690,7 +8714,7 @@
         <v>308</v>
       </c>
       <c r="C187" s="27" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="D187" s="25"/>
       <c r="E187" s="25" t="s">
@@ -8715,7 +8739,7 @@
         <v>308</v>
       </c>
       <c r="C188" s="27" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="D188" s="25"/>
       <c r="E188" s="25" t="s">
@@ -8739,8 +8763,8 @@
       <c r="B189" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="C189" s="27" t="s">
-        <v>490</v>
+      <c r="C189" s="16" t="s">
+        <v>561</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25" t="s">
@@ -8765,7 +8789,7 @@
         <v>308</v>
       </c>
       <c r="C190" s="27" t="s">
-        <v>491</v>
+        <v>471</v>
       </c>
       <c r="D190" s="25"/>
       <c r="E190" s="25" t="s">
@@ -8790,7 +8814,7 @@
         <v>308</v>
       </c>
       <c r="C191" s="27" t="s">
-        <v>492</v>
+        <v>472</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25" t="s">
@@ -8815,7 +8839,7 @@
         <v>309</v>
       </c>
       <c r="C192" s="27" t="s">
-        <v>493</v>
+        <v>473</v>
       </c>
       <c r="D192" s="25"/>
       <c r="E192" s="25" t="s">
@@ -8839,8 +8863,8 @@
       <c r="B193" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="C193" s="27" t="s">
-        <v>494</v>
+      <c r="C193" s="16" t="s">
+        <v>562</v>
       </c>
       <c r="D193" s="25"/>
       <c r="E193" s="25" t="s">
@@ -8865,7 +8889,7 @@
         <v>309</v>
       </c>
       <c r="C194" s="27" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="D194" s="25"/>
       <c r="E194" s="25" t="s">
@@ -8890,7 +8914,7 @@
         <v>310</v>
       </c>
       <c r="C195" s="27" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="D195" s="25"/>
       <c r="E195" s="25" t="s">
@@ -8914,8 +8938,8 @@
       <c r="B196" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="C196" s="27" t="s">
-        <v>497</v>
+      <c r="C196" s="16" t="s">
+        <v>563</v>
       </c>
       <c r="D196" s="25"/>
       <c r="E196" s="25" t="s">
@@ -8940,7 +8964,7 @@
         <v>310</v>
       </c>
       <c r="C197" s="27" t="s">
-        <v>498</v>
+        <v>476</v>
       </c>
       <c r="D197" s="25"/>
       <c r="E197" s="25" t="s">
@@ -8965,7 +8989,7 @@
         <v>310</v>
       </c>
       <c r="C198" s="27" t="s">
-        <v>499</v>
+        <v>477</v>
       </c>
       <c r="D198" s="25"/>
       <c r="E198" s="25" t="s">
@@ -8990,7 +9014,7 @@
         <v>310</v>
       </c>
       <c r="C199" s="27" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="D199" s="25"/>
       <c r="E199" s="25" t="s">
@@ -9015,7 +9039,7 @@
         <v>310</v>
       </c>
       <c r="C200" s="27" t="s">
-        <v>501</v>
+        <v>479</v>
       </c>
       <c r="D200" s="25"/>
       <c r="E200" s="25" t="s">
@@ -9040,7 +9064,7 @@
         <v>310</v>
       </c>
       <c r="C201" s="27" t="s">
-        <v>502</v>
+        <v>480</v>
       </c>
       <c r="D201" s="25"/>
       <c r="E201" s="25" t="s">
@@ -9065,7 +9089,7 @@
         <v>311</v>
       </c>
       <c r="C202" s="27" t="s">
-        <v>503</v>
+        <v>481</v>
       </c>
       <c r="D202" s="25"/>
       <c r="E202" s="25" t="s">
@@ -9090,7 +9114,7 @@
         <v>311</v>
       </c>
       <c r="C203" s="27" t="s">
-        <v>504</v>
+        <v>482</v>
       </c>
       <c r="D203" s="25"/>
       <c r="E203" s="25" t="s">
@@ -9114,8 +9138,8 @@
       <c r="B204" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="C204" s="27" t="s">
-        <v>505</v>
+      <c r="C204" s="16" t="s">
+        <v>564</v>
       </c>
       <c r="D204" s="25"/>
       <c r="E204" s="25" t="s">
@@ -9140,7 +9164,7 @@
         <v>311</v>
       </c>
       <c r="C205" s="27" t="s">
-        <v>506</v>
+        <v>483</v>
       </c>
       <c r="D205" s="25"/>
       <c r="E205" s="25" t="s">
@@ -9165,7 +9189,7 @@
         <v>311</v>
       </c>
       <c r="C206" s="27" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
       <c r="D206" s="25"/>
       <c r="E206" s="25" t="s">
@@ -9189,8 +9213,8 @@
       <c r="B207" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="C207" s="27" t="s">
-        <v>508</v>
+      <c r="C207" s="16" t="s">
+        <v>565</v>
       </c>
       <c r="D207" s="25"/>
       <c r="E207" s="25" t="s">
@@ -9215,7 +9239,7 @@
         <v>311</v>
       </c>
       <c r="C208" s="27" t="s">
-        <v>509</v>
+        <v>485</v>
       </c>
       <c r="D208" s="25"/>
       <c r="E208" s="25" t="s">
@@ -9240,7 +9264,7 @@
         <v>311</v>
       </c>
       <c r="C209" s="27" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="D209" s="25"/>
       <c r="E209" s="25" t="s">
@@ -9265,7 +9289,7 @@
         <v>311</v>
       </c>
       <c r="C210" s="27" t="s">
-        <v>511</v>
+        <v>487</v>
       </c>
       <c r="D210" s="25"/>
       <c r="E210" s="25" t="s">
@@ -9290,7 +9314,7 @@
         <v>311</v>
       </c>
       <c r="C211" s="27" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
       <c r="D211" s="25"/>
       <c r="E211" s="25" t="s">
@@ -9315,7 +9339,7 @@
         <v>311</v>
       </c>
       <c r="C212" s="27" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
       <c r="D212" s="25"/>
       <c r="E212" s="25" t="s">
@@ -9340,7 +9364,7 @@
         <v>311</v>
       </c>
       <c r="C213" s="27" t="s">
-        <v>514</v>
+        <v>490</v>
       </c>
       <c r="D213" s="25"/>
       <c r="E213" s="25" t="s">
@@ -9365,7 +9389,7 @@
         <v>311</v>
       </c>
       <c r="C214" s="27" t="s">
-        <v>515</v>
+        <v>491</v>
       </c>
       <c r="D214" s="25"/>
       <c r="E214" s="25" t="s">
@@ -9390,7 +9414,7 @@
         <v>311</v>
       </c>
       <c r="C215" s="27" t="s">
-        <v>516</v>
+        <v>492</v>
       </c>
       <c r="D215" s="25"/>
       <c r="E215" s="25" t="s">
@@ -9415,7 +9439,7 @@
         <v>311</v>
       </c>
       <c r="C216" s="27" t="s">
-        <v>517</v>
+        <v>493</v>
       </c>
       <c r="D216" s="25"/>
       <c r="E216" s="25" t="s">
@@ -9440,7 +9464,7 @@
         <v>311</v>
       </c>
       <c r="C217" s="27" t="s">
-        <v>518</v>
+        <v>494</v>
       </c>
       <c r="D217" s="25"/>
       <c r="E217" s="25" t="s">
@@ -9465,7 +9489,7 @@
         <v>311</v>
       </c>
       <c r="C218" s="27" t="s">
-        <v>519</v>
+        <v>495</v>
       </c>
       <c r="D218" s="25"/>
       <c r="E218" s="25" t="s">
@@ -9490,7 +9514,7 @@
         <v>311</v>
       </c>
       <c r="C219" s="27" t="s">
-        <v>520</v>
+        <v>496</v>
       </c>
       <c r="D219" s="25"/>
       <c r="E219" s="25" t="s">
@@ -9515,7 +9539,7 @@
         <v>312</v>
       </c>
       <c r="C220" s="27" t="s">
-        <v>521</v>
+        <v>497</v>
       </c>
       <c r="D220" s="25"/>
       <c r="E220" s="25" t="s">
@@ -9540,7 +9564,7 @@
         <v>312</v>
       </c>
       <c r="C221" s="27" t="s">
-        <v>522</v>
+        <v>498</v>
       </c>
       <c r="D221" s="25"/>
       <c r="E221" s="25" t="s">
@@ -9565,7 +9589,7 @@
         <v>313</v>
       </c>
       <c r="C222" s="27" t="s">
-        <v>523</v>
+        <v>499</v>
       </c>
       <c r="D222" s="25"/>
       <c r="E222" s="25" t="s">
@@ -9590,7 +9614,7 @@
         <v>313</v>
       </c>
       <c r="C223" s="27" t="s">
-        <v>524</v>
+        <v>500</v>
       </c>
       <c r="D223" s="25"/>
       <c r="E223" s="25" t="s">
@@ -9615,7 +9639,7 @@
         <v>313</v>
       </c>
       <c r="C224" s="27" t="s">
-        <v>525</v>
+        <v>501</v>
       </c>
       <c r="D224" s="25"/>
       <c r="E224" s="25" t="s">
@@ -9640,7 +9664,7 @@
         <v>313</v>
       </c>
       <c r="C225" s="27" t="s">
-        <v>526</v>
+        <v>502</v>
       </c>
       <c r="D225" s="25"/>
       <c r="E225" s="25" t="s">
@@ -9665,7 +9689,7 @@
         <v>313</v>
       </c>
       <c r="C226" s="27" t="s">
-        <v>527</v>
+        <v>503</v>
       </c>
       <c r="D226" s="25"/>
       <c r="E226" s="25" t="s">
@@ -9690,7 +9714,7 @@
         <v>313</v>
       </c>
       <c r="C227" s="27" t="s">
-        <v>528</v>
+        <v>504</v>
       </c>
       <c r="D227" s="25"/>
       <c r="E227" s="25" t="s">
@@ -9715,7 +9739,7 @@
         <v>313</v>
       </c>
       <c r="C228" s="27" t="s">
-        <v>529</v>
+        <v>505</v>
       </c>
       <c r="D228" s="25"/>
       <c r="E228" s="25" t="s">
@@ -9740,7 +9764,7 @@
         <v>313</v>
       </c>
       <c r="C229" s="27" t="s">
-        <v>530</v>
+        <v>506</v>
       </c>
       <c r="D229" s="25"/>
       <c r="E229" s="25" t="s">
@@ -9765,7 +9789,7 @@
         <v>313</v>
       </c>
       <c r="C230" s="27" t="s">
-        <v>531</v>
+        <v>507</v>
       </c>
       <c r="D230" s="25"/>
       <c r="E230" s="25" t="s">
@@ -9790,7 +9814,7 @@
         <v>313</v>
       </c>
       <c r="C231" s="27" t="s">
-        <v>532</v>
+        <v>508</v>
       </c>
       <c r="D231" s="25"/>
       <c r="E231" s="25" t="s">
@@ -9815,7 +9839,7 @@
         <v>313</v>
       </c>
       <c r="C232" s="27" t="s">
-        <v>533</v>
+        <v>509</v>
       </c>
       <c r="D232" s="25"/>
       <c r="E232" s="25" t="s">
@@ -9840,7 +9864,7 @@
         <v>313</v>
       </c>
       <c r="C233" s="27" t="s">
-        <v>534</v>
+        <v>510</v>
       </c>
       <c r="D233" s="25"/>
       <c r="E233" s="25" t="s">
@@ -9865,7 +9889,7 @@
         <v>313</v>
       </c>
       <c r="C234" s="27" t="s">
-        <v>535</v>
+        <v>511</v>
       </c>
       <c r="D234" s="25"/>
       <c r="E234" s="25" t="s">
@@ -9890,7 +9914,7 @@
         <v>313</v>
       </c>
       <c r="C235" s="27" t="s">
-        <v>536</v>
+        <v>512</v>
       </c>
       <c r="D235" s="25"/>
       <c r="E235" s="25" t="s">
@@ -9915,7 +9939,7 @@
         <v>313</v>
       </c>
       <c r="C236" s="27" t="s">
-        <v>537</v>
+        <v>513</v>
       </c>
       <c r="D236" s="25"/>
       <c r="E236" s="25" t="s">
@@ -9940,7 +9964,7 @@
         <v>314</v>
       </c>
       <c r="C237" s="27" t="s">
-        <v>538</v>
+        <v>514</v>
       </c>
       <c r="D237" s="25"/>
       <c r="E237" s="25" t="s">
@@ -9965,7 +9989,7 @@
         <v>314</v>
       </c>
       <c r="C238" s="27" t="s">
-        <v>539</v>
+        <v>515</v>
       </c>
       <c r="D238" s="25"/>
       <c r="E238" s="25" t="s">
@@ -9982,7 +10006,7 @@
       </c>
       <c r="I238" s="27"/>
     </row>
-    <row r="239" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" s="25" t="s">
         <v>259</v>
       </c>
@@ -9990,10 +10014,10 @@
         <v>314</v>
       </c>
       <c r="C239" s="27" t="s">
-        <v>540</v>
+        <v>516</v>
       </c>
       <c r="D239" s="25" t="s">
-        <v>553</v>
+        <v>529</v>
       </c>
       <c r="E239" s="25" t="s">
         <v>22</v>
@@ -10008,7 +10032,7 @@
         <v>21</v>
       </c>
       <c r="I239" s="27" t="s">
-        <v>557</v>
+        <v>533</v>
       </c>
     </row>
     <row r="240" spans="1:9" ht="240" x14ac:dyDescent="0.25">
@@ -10019,10 +10043,10 @@
         <v>314</v>
       </c>
       <c r="C240" s="27" t="s">
-        <v>541</v>
+        <v>517</v>
       </c>
       <c r="D240" s="25" t="s">
-        <v>554</v>
+        <v>530</v>
       </c>
       <c r="E240" s="25" t="s">
         <v>22</v>
@@ -10037,7 +10061,7 @@
         <v>20</v>
       </c>
       <c r="I240" s="27" t="s">
-        <v>557</v>
+        <v>533</v>
       </c>
     </row>
     <row r="241" spans="1:9" ht="255" x14ac:dyDescent="0.25">
@@ -10048,10 +10072,10 @@
         <v>314</v>
       </c>
       <c r="C241" s="27" t="s">
-        <v>542</v>
+        <v>518</v>
       </c>
       <c r="D241" s="25" t="s">
-        <v>554</v>
+        <v>530</v>
       </c>
       <c r="E241" s="25" t="s">
         <v>22</v>
@@ -10075,10 +10099,10 @@
         <v>314</v>
       </c>
       <c r="C242" s="27" t="s">
-        <v>543</v>
+        <v>519</v>
       </c>
       <c r="D242" s="25" t="s">
-        <v>555</v>
+        <v>531</v>
       </c>
       <c r="E242" s="25" t="s">
         <v>22</v>
@@ -10102,10 +10126,10 @@
         <v>314</v>
       </c>
       <c r="C243" s="27" t="s">
-        <v>544</v>
+        <v>520</v>
       </c>
       <c r="D243" s="25" t="s">
-        <v>555</v>
+        <v>531</v>
       </c>
       <c r="E243" s="25" t="s">
         <v>22</v>
@@ -10129,7 +10153,7 @@
         <v>315</v>
       </c>
       <c r="C244" s="27" t="s">
-        <v>545</v>
+        <v>521</v>
       </c>
       <c r="D244" s="25"/>
       <c r="E244" s="25" t="s">
@@ -10154,7 +10178,7 @@
         <v>316</v>
       </c>
       <c r="C245" s="28" t="s">
-        <v>562</v>
+        <v>538</v>
       </c>
       <c r="D245" s="25"/>
       <c r="E245" s="25" t="s">
@@ -10179,7 +10203,7 @@
         <v>317</v>
       </c>
       <c r="C246" s="28" t="s">
-        <v>561</v>
+        <v>537</v>
       </c>
       <c r="D246" s="25"/>
       <c r="E246" s="25" t="s">
@@ -10204,7 +10228,7 @@
         <v>318</v>
       </c>
       <c r="C247" s="27" t="s">
-        <v>546</v>
+        <v>522</v>
       </c>
       <c r="D247" s="25"/>
       <c r="E247" s="25" t="s">
@@ -10229,7 +10253,7 @@
         <v>318</v>
       </c>
       <c r="C248" s="27" t="s">
-        <v>547</v>
+        <v>523</v>
       </c>
       <c r="D248" s="25"/>
       <c r="E248" s="25" t="s">
@@ -10254,7 +10278,7 @@
         <v>318</v>
       </c>
       <c r="C249" s="27" t="s">
-        <v>548</v>
+        <v>524</v>
       </c>
       <c r="D249" s="25"/>
       <c r="E249" s="25" t="s">
@@ -10279,7 +10303,7 @@
         <v>319</v>
       </c>
       <c r="C250" s="27" t="s">
-        <v>549</v>
+        <v>525</v>
       </c>
       <c r="D250" s="25"/>
       <c r="E250" s="25" t="s">
@@ -10304,7 +10328,7 @@
         <v>319</v>
       </c>
       <c r="C251" s="27" t="s">
-        <v>550</v>
+        <v>526</v>
       </c>
       <c r="D251" s="25"/>
       <c r="E251" s="25" t="s">
@@ -10329,7 +10353,7 @@
         <v>319</v>
       </c>
       <c r="C252" s="27" t="s">
-        <v>551</v>
+        <v>527</v>
       </c>
       <c r="D252" s="25"/>
       <c r="E252" s="25" t="s">
@@ -10354,7 +10378,7 @@
         <v>320</v>
       </c>
       <c r="C253" s="27" t="s">
-        <v>552</v>
+        <v>528</v>
       </c>
       <c r="D253" s="25"/>
       <c r="E253" s="25" t="s">
@@ -10492,7 +10516,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 C3 B244:B255 B10:B243" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B244:B255 B10:B243" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
[MS-OXWSBTRF] Fix watchman error
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSBTRF/MS-OXWSBTRF_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSBTRF/MS-OXWSBTRF_RequirementSpecification.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\E16 EWS update\20160310_BTRF\Docs\MS-OXWSBTRF\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
   </bookViews>
@@ -292,80 +287,6 @@
         <family val="2"/>
       </rPr>
       <t>: Statements are required for interoperability.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Test Case: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Indicates that a requirement will be captured in Test Case code.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Adapter: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Indicates that a requirement will be captured in Adapter code.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Non-testable: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Indicates that a requirement is not testable. It can not be verified by generating and observing data on the wire.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Unverified: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Indicates that a requirement is verifiable, but choose not to test because of cost or other reason.</t>
     </r>
   </si>
   <si>
@@ -2789,19 +2710,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In tns:ExportItemsSoapOut Message]The type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.3.12).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In tns:ExportItemsSoapOut Message][If the request is unsuccessful]The ResponseCode element of the ExportItemsResponseMessage element is set to a value of the ResponseCodeType simple type, as specified in [MS-OXWSCDATA] section 2.2.5.24.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>[In m:ExportItemsResponseMessageType Complex Type]The ExportItemsResponseMessageType complex type extends the ResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.67.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In m:ExportItemsResponseMessageType Complex Type]The type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2833,10 +2746,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In tns:UploadItemsSoapOut Message][If the request UploadItems request is unsuccessful]The ResponseCode element of the UploadItemsResponseMessage element is set to a value of the ResponseCodeType simple type, as specified in [MS-OXWSCDATA] section 2.2.5.24.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In tns:UploadItemsSoapOut Message]The Element/type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.3.12).</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2845,23 +2754,129 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>[In m:UploadItemsResponseType Complex Type]The UploadItemsResponseType complex type extends the BaseResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.18.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:UploadItemsType Complex Type]The UploadItemsType complex type extends the BaseRequestType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.17.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:UploadItemType Complex Type]The Type of ParentFolderId is t:FolderIdType ([MS-OXWSCDATA] section 2.2.4.36).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:UploadItemType Complex Type]The Type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Case: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Indicates that a requirement will be captured in Test Case code.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Adapter: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Indicates that a requirement will be captured in Adapter code.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Non-testable: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Indicates that a requirement is not testable. It can not be verified by generating and observing data on the wire.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Unverified: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Indicates that a requirement is verifiable, but choose not to test because of cost or other reason.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Message Deserialization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Indicates that a requirement is verified when deserializing the response message.</t>
+    </r>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapOut Message]The type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.3.12).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In m:ExportItemsResponseMessageType Complex Type]The type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>[In m:UploadItemsResponseMessageType Complex Type]The Type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In m:UploadItemsResponseType Complex Type]The UploadItemsResponseType complex type extends the BaseResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.18.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In m:UploadItemsType Complex Type]The UploadItemsType complex type extends the BaseRequestType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.17.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In m:UploadItemType Complex Type]The Type of ParentFolderId is t:FolderIdType ([MS-OXWSCDATA] section 2.2.4.36).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In m:UploadItemType Complex Type]The Type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
+    <t>[In tns:UploadItemsSoapOut Message][If the request UploadItems request is unsuccessful]The ResponseCode element of the UploadItemsResponseMessage element is set to a value of the ResponseCodeType simple type, as specified in [MS-OXWSCDATA] section 2.2.5.24.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3113,7 +3128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3275,6 +3290,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4190,7 +4208,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -4202,7 +4220,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4306,7 +4324,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C8" s="55"/>
       <c r="D8" s="55"/>
@@ -4357,7 +4375,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C11" s="61"/>
       <c r="D11" s="47"/>
@@ -4462,20 +4480,20 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:13" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="48"/>
+        <v>561</v>
+      </c>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -4484,7 +4502,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
@@ -4529,13 +4547,13 @@
     </row>
     <row r="20" spans="1:13" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18" t="s">
@@ -4554,13 +4572,13 @@
     </row>
     <row r="21" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18" t="s">
@@ -4579,13 +4597,13 @@
     </row>
     <row r="22" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18" t="s">
@@ -4604,13 +4622,13 @@
     </row>
     <row r="23" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18" t="s">
@@ -4629,13 +4647,13 @@
     </row>
     <row r="24" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18" t="s">
@@ -4654,13 +4672,13 @@
     </row>
     <row r="25" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18" t="s">
@@ -4679,13 +4697,13 @@
     </row>
     <row r="26" spans="1:13" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18" t="s">
@@ -4704,13 +4722,13 @@
     </row>
     <row r="27" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18" t="s">
@@ -4729,13 +4747,13 @@
     </row>
     <row r="28" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A28" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="18" t="s">
@@ -4754,13 +4772,13 @@
     </row>
     <row r="29" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18" t="s">
@@ -4779,13 +4797,13 @@
     </row>
     <row r="30" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18" t="s">
@@ -4801,18 +4819,18 @@
         <v>17</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18" t="s">
@@ -4831,13 +4849,13 @@
     </row>
     <row r="32" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18" t="s">
@@ -4856,13 +4874,13 @@
     </row>
     <row r="33" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A33" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18" t="s">
@@ -4881,13 +4899,13 @@
     </row>
     <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="25" t="s">
@@ -4906,13 +4924,13 @@
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="25" t="s">
@@ -4931,13 +4949,13 @@
     </row>
     <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="25" t="s">
@@ -4956,13 +4974,13 @@
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="25" t="s">
@@ -4981,13 +4999,13 @@
     </row>
     <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="25" t="s">
@@ -5006,13 +5024,13 @@
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="25" t="s">
@@ -5031,13 +5049,13 @@
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="25" t="s">
@@ -5056,13 +5074,13 @@
     </row>
     <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D41" s="25"/>
       <c r="E41" s="25" t="s">
@@ -5081,13 +5099,13 @@
     </row>
     <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D42" s="25"/>
       <c r="E42" s="25" t="s">
@@ -5106,13 +5124,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D43" s="25"/>
       <c r="E43" s="25" t="s">
@@ -5131,13 +5149,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="25" t="s">
@@ -5156,13 +5174,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D45" s="25"/>
       <c r="E45" s="25" t="s">
@@ -5181,13 +5199,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D46" s="25"/>
       <c r="E46" s="25" t="s">
@@ -5206,13 +5224,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="25" t="s">
@@ -5231,13 +5249,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D48" s="25"/>
       <c r="E48" s="25" t="s">
@@ -5256,13 +5274,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="25" t="s">
@@ -5281,13 +5299,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D50" s="25"/>
       <c r="E50" s="25" t="s">
@@ -5306,13 +5324,13 @@
     </row>
     <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="25" t="s">
@@ -5331,13 +5349,13 @@
     </row>
     <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D52" s="25"/>
       <c r="E52" s="25" t="s">
@@ -5356,13 +5374,13 @@
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D53" s="25"/>
       <c r="E53" s="25" t="s">
@@ -5381,13 +5399,13 @@
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="25" t="s">
@@ -5406,13 +5424,13 @@
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D55" s="25"/>
       <c r="E55" s="25" t="s">
@@ -5431,13 +5449,13 @@
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D56" s="25"/>
       <c r="E56" s="25" t="s">
@@ -5456,13 +5474,13 @@
     </row>
     <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D57" s="25"/>
       <c r="E57" s="25" t="s">
@@ -5481,13 +5499,13 @@
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D58" s="25"/>
       <c r="E58" s="25" t="s">
@@ -5506,13 +5524,13 @@
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B59" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D59" s="25"/>
       <c r="E59" s="25" t="s">
@@ -5531,13 +5549,13 @@
     </row>
     <row r="60" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B60" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D60" s="25"/>
       <c r="E60" s="25" t="s">
@@ -5556,13 +5574,13 @@
     </row>
     <row r="61" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D61" s="25"/>
       <c r="E61" s="25" t="s">
@@ -5578,18 +5596,18 @@
         <v>17</v>
       </c>
       <c r="I61" s="27" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D62" s="25"/>
       <c r="E62" s="25" t="s">
@@ -5608,13 +5626,13 @@
     </row>
     <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D63" s="25"/>
       <c r="E63" s="25" t="s">
@@ -5633,13 +5651,13 @@
     </row>
     <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D64" s="25"/>
       <c r="E64" s="25" t="s">
@@ -5658,13 +5676,13 @@
     </row>
     <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C65" s="27" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D65" s="25"/>
       <c r="E65" s="25" t="s">
@@ -5683,13 +5701,13 @@
     </row>
     <row r="66" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D66" s="25"/>
       <c r="E66" s="25" t="s">
@@ -5708,13 +5726,13 @@
     </row>
     <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D67" s="25"/>
       <c r="E67" s="25" t="s">
@@ -5733,13 +5751,13 @@
     </row>
     <row r="68" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25" t="s">
@@ -5758,13 +5776,13 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D69" s="25"/>
       <c r="E69" s="25" t="s">
@@ -5783,13 +5801,13 @@
     </row>
     <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D70" s="25"/>
       <c r="E70" s="25" t="s">
@@ -5808,13 +5826,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C71" s="27" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D71" s="25"/>
       <c r="E71" s="25" t="s">
@@ -5833,13 +5851,13 @@
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D72" s="25"/>
       <c r="E72" s="25" t="s">
@@ -5858,13 +5876,13 @@
     </row>
     <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C73" s="27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D73" s="25"/>
       <c r="E73" s="25" t="s">
@@ -5883,13 +5901,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D74" s="25"/>
       <c r="E74" s="25" t="s">
@@ -5908,13 +5926,13 @@
     </row>
     <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D75" s="25"/>
       <c r="E75" s="25" t="s">
@@ -5933,13 +5951,13 @@
     </row>
     <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C76" s="27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D76" s="25"/>
       <c r="E76" s="25" t="s">
@@ -5958,13 +5976,13 @@
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D77" s="25"/>
       <c r="E77" s="25" t="s">
@@ -5983,13 +6001,13 @@
     </row>
     <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C78" s="27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D78" s="25"/>
       <c r="E78" s="25" t="s">
@@ -6008,13 +6026,13 @@
     </row>
     <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D79" s="25"/>
       <c r="E79" s="25" t="s">
@@ -6033,13 +6051,13 @@
     </row>
     <row r="80" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C80" s="27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D80" s="25"/>
       <c r="E80" s="25" t="s">
@@ -6058,13 +6076,13 @@
     </row>
     <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C81" s="27" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D81" s="25"/>
       <c r="E81" s="25" t="s">
@@ -6083,13 +6101,13 @@
     </row>
     <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C82" s="27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D82" s="25"/>
       <c r="E82" s="25" t="s">
@@ -6108,13 +6126,13 @@
     </row>
     <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C83" s="27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D83" s="25"/>
       <c r="E83" s="25" t="s">
@@ -6133,13 +6151,13 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D84" s="25"/>
       <c r="E84" s="25" t="s">
@@ -6158,13 +6176,13 @@
     </row>
     <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>548</v>
+        <v>562</v>
       </c>
       <c r="D85" s="25"/>
       <c r="E85" s="25" t="s">
@@ -6183,13 +6201,13 @@
     </row>
     <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C86" s="27" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D86" s="25"/>
       <c r="E86" s="25" t="s">
@@ -6208,13 +6226,13 @@
     </row>
     <row r="87" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D87" s="25"/>
       <c r="E87" s="25" t="s">
@@ -6233,13 +6251,13 @@
     </row>
     <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D88" s="25"/>
       <c r="E88" s="25" t="s">
@@ -6258,13 +6276,13 @@
     </row>
     <row r="89" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D89" s="25"/>
       <c r="E89" s="25" t="s">
@@ -6283,13 +6301,13 @@
     </row>
     <row r="90" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D90" s="25"/>
       <c r="E90" s="25" t="s">
@@ -6308,13 +6326,13 @@
     </row>
     <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C91" s="27" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D91" s="25"/>
       <c r="E91" s="25" t="s">
@@ -6333,13 +6351,13 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C92" s="27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D92" s="25"/>
       <c r="E92" s="25" t="s">
@@ -6358,13 +6376,13 @@
     </row>
     <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C93" s="27" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D93" s="25"/>
       <c r="E93" s="25" t="s">
@@ -6383,13 +6401,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C94" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D94" s="25"/>
       <c r="E94" s="25" t="s">
@@ -6408,13 +6426,13 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C95" s="27" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D95" s="25"/>
       <c r="E95" s="25" t="s">
@@ -6433,13 +6451,13 @@
     </row>
     <row r="96" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C96" s="27" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D96" s="25"/>
       <c r="E96" s="25" t="s">
@@ -6458,13 +6476,13 @@
     </row>
     <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C97" s="27" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D97" s="25"/>
       <c r="E97" s="25" t="s">
@@ -6483,13 +6501,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C98" s="27" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D98" s="25"/>
       <c r="E98" s="25" t="s">
@@ -6508,13 +6526,13 @@
     </row>
     <row r="99" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C99" s="27" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D99" s="25"/>
       <c r="E99" s="25" t="s">
@@ -6533,13 +6551,13 @@
     </row>
     <row r="100" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B100" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C100" s="27" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D100" s="25"/>
       <c r="E100" s="25" t="s">
@@ -6558,13 +6576,13 @@
     </row>
     <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C101" s="27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D101" s="25"/>
       <c r="E101" s="25" t="s">
@@ -6583,13 +6601,13 @@
     </row>
     <row r="102" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B102" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C102" s="27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D102" s="25"/>
       <c r="E102" s="25" t="s">
@@ -6608,13 +6626,13 @@
     </row>
     <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C103" s="27" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D103" s="25"/>
       <c r="E103" s="25" t="s">
@@ -6633,13 +6651,13 @@
     </row>
     <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C104" s="27" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D104" s="25"/>
       <c r="E104" s="25" t="s">
@@ -6658,13 +6676,13 @@
     </row>
     <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C105" s="27" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D105" s="25"/>
       <c r="E105" s="25" t="s">
@@ -6683,13 +6701,13 @@
     </row>
     <row r="106" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C106" s="16" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D106" s="25"/>
       <c r="E106" s="25" t="s">
@@ -6708,13 +6726,13 @@
     </row>
     <row r="107" spans="1:9" ht="330" x14ac:dyDescent="0.25">
       <c r="A107" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C107" s="27" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D107" s="25"/>
       <c r="E107" s="25" t="s">
@@ -6733,13 +6751,13 @@
     </row>
     <row r="108" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C108" s="27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D108" s="25"/>
       <c r="E108" s="25" t="s">
@@ -6758,13 +6776,13 @@
     </row>
     <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C109" s="16" t="s">
-        <v>551</v>
+        <v>563</v>
       </c>
       <c r="D109" s="25"/>
       <c r="E109" s="25" t="s">
@@ -6783,13 +6801,13 @@
     </row>
     <row r="110" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C110" s="27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D110" s="25"/>
       <c r="E110" s="25" t="s">
@@ -6808,13 +6826,13 @@
     </row>
     <row r="111" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C111" s="27" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D111" s="25"/>
       <c r="E111" s="25" t="s">
@@ -6833,13 +6851,13 @@
     </row>
     <row r="112" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C112" s="27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D112" s="25"/>
       <c r="E112" s="25" t="s">
@@ -6858,13 +6876,13 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C113" s="27" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D113" s="25"/>
       <c r="E113" s="25" t="s">
@@ -6883,13 +6901,13 @@
     </row>
     <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B114" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C114" s="27" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D114" s="25"/>
       <c r="E114" s="25" t="s">
@@ -6908,13 +6926,13 @@
     </row>
     <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B115" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C115" s="27" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D115" s="25"/>
       <c r="E115" s="25" t="s">
@@ -6933,13 +6951,13 @@
     </row>
     <row r="116" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="25" t="s">
@@ -6958,13 +6976,13 @@
     </row>
     <row r="117" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B117" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C117" s="27" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="25" t="s">
@@ -6983,13 +7001,13 @@
     </row>
     <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B118" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C118" s="27" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="25" t="s">
@@ -7008,13 +7026,13 @@
     </row>
     <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B119" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="D119" s="25"/>
       <c r="E119" s="25" t="s">
@@ -7033,13 +7051,13 @@
     </row>
     <row r="120" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A120" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B120" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C120" s="27" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D120" s="25"/>
       <c r="E120" s="25" t="s">
@@ -7058,13 +7076,13 @@
     </row>
     <row r="121" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B121" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C121" s="27" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="25" t="s">
@@ -7083,13 +7101,13 @@
     </row>
     <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B122" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C122" s="27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D122" s="25"/>
       <c r="E122" s="25" t="s">
@@ -7108,13 +7126,13 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B123" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C123" s="27" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D123" s="25"/>
       <c r="E123" s="25" t="s">
@@ -7133,13 +7151,13 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B124" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C124" s="27" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D124" s="25"/>
       <c r="E124" s="25" t="s">
@@ -7158,13 +7176,13 @@
     </row>
     <row r="125" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A125" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B125" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C125" s="27" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D125" s="25"/>
       <c r="E125" s="25" t="s">
@@ -7183,13 +7201,13 @@
     </row>
     <row r="126" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B126" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C126" s="27" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D126" s="25"/>
       <c r="E126" s="25" t="s">
@@ -7208,13 +7226,13 @@
     </row>
     <row r="127" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B127" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C127" s="16" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D127" s="25"/>
       <c r="E127" s="25" t="s">
@@ -7233,13 +7251,13 @@
     </row>
     <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B128" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C128" s="27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D128" s="25"/>
       <c r="E128" s="25" t="s">
@@ -7258,13 +7276,13 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B129" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C129" s="27" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="25" t="s">
@@ -7283,13 +7301,13 @@
     </row>
     <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B130" s="26" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C130" s="27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D130" s="25"/>
       <c r="E130" s="25" t="s">
@@ -7308,13 +7326,13 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B131" s="26" t="s">
         <v>32</v>
       </c>
       <c r="C131" s="27" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D131" s="25"/>
       <c r="E131" s="25" t="s">
@@ -7333,13 +7351,13 @@
     </row>
     <row r="132" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A132" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B132" s="26" t="s">
         <v>32</v>
       </c>
       <c r="C132" s="27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D132" s="25"/>
       <c r="E132" s="25" t="s">
@@ -7358,13 +7376,13 @@
     </row>
     <row r="133" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A133" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B133" s="26" t="s">
         <v>32</v>
       </c>
       <c r="C133" s="27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D133" s="25"/>
       <c r="E133" s="25" t="s">
@@ -7383,13 +7401,13 @@
     </row>
     <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B134" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C134" s="27" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D134" s="25"/>
       <c r="E134" s="25" t="s">
@@ -7408,13 +7426,13 @@
     </row>
     <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A135" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B135" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C135" s="27" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D135" s="25"/>
       <c r="E135" s="25" t="s">
@@ -7433,13 +7451,13 @@
     </row>
     <row r="136" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B136" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C136" s="27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D136" s="25"/>
       <c r="E136" s="25" t="s">
@@ -7458,13 +7476,13 @@
     </row>
     <row r="137" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B137" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C137" s="27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D137" s="25"/>
       <c r="E137" s="25" t="s">
@@ -7483,13 +7501,13 @@
     </row>
     <row r="138" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B138" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C138" s="27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D138" s="25"/>
       <c r="E138" s="25" t="s">
@@ -7508,13 +7526,13 @@
     </row>
     <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B139" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C139" s="27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D139" s="25"/>
       <c r="E139" s="25" t="s">
@@ -7533,13 +7551,13 @@
     </row>
     <row r="140" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B140" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C140" s="27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D140" s="25"/>
       <c r="E140" s="25" t="s">
@@ -7558,13 +7576,13 @@
     </row>
     <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B141" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C141" s="27" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D141" s="25"/>
       <c r="E141" s="25" t="s">
@@ -7583,13 +7601,13 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B142" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C142" s="27" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D142" s="25"/>
       <c r="E142" s="25" t="s">
@@ -7608,13 +7626,13 @@
     </row>
     <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B143" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C143" s="16" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D143" s="25"/>
       <c r="E143" s="25" t="s">
@@ -7633,13 +7651,13 @@
     </row>
     <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B144" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C144" s="27" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D144" s="25"/>
       <c r="E144" s="25" t="s">
@@ -7658,13 +7676,13 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B145" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C145" s="27" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="25" t="s">
@@ -7683,13 +7701,13 @@
     </row>
     <row r="146" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B146" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C146" s="16" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="D146" s="25"/>
       <c r="E146" s="25" t="s">
@@ -7708,13 +7726,13 @@
     </row>
     <row r="147" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B147" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C147" s="27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D147" s="25"/>
       <c r="E147" s="25" t="s">
@@ -7733,13 +7751,13 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B148" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C148" s="27" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D148" s="25"/>
       <c r="E148" s="25" t="s">
@@ -7758,13 +7776,13 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B149" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C149" s="27" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="25" t="s">
@@ -7783,13 +7801,13 @@
     </row>
     <row r="150" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B150" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C150" s="16" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D150" s="25"/>
       <c r="E150" s="25" t="s">
@@ -7808,13 +7826,13 @@
     </row>
     <row r="151" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B151" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C151" s="27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D151" s="25"/>
       <c r="E151" s="25" t="s">
@@ -7833,13 +7851,13 @@
     </row>
     <row r="152" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A152" s="25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B152" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C152" s="27" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D152" s="25"/>
       <c r="E152" s="25" t="s">
@@ -7858,13 +7876,13 @@
     </row>
     <row r="153" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B153" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C153" s="27" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D153" s="25"/>
       <c r="E153" s="25" t="s">
@@ -7883,13 +7901,13 @@
     </row>
     <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B154" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C154" s="27" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D154" s="25"/>
       <c r="E154" s="25" t="s">
@@ -7908,13 +7926,13 @@
     </row>
     <row r="155" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B155" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C155" s="27" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D155" s="25"/>
       <c r="E155" s="25" t="s">
@@ -7933,13 +7951,13 @@
     </row>
     <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B156" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C156" s="27" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D156" s="25"/>
       <c r="E156" s="25" t="s">
@@ -7958,13 +7976,13 @@
     </row>
     <row r="157" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B157" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C157" s="16" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D157" s="25"/>
       <c r="E157" s="25" t="s">
@@ -7983,13 +8001,13 @@
     </row>
     <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B158" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C158" s="27" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D158" s="25"/>
       <c r="E158" s="25" t="s">
@@ -8008,13 +8026,13 @@
     </row>
     <row r="159" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A159" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B159" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C159" s="27" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D159" s="25"/>
       <c r="E159" s="25" t="s">
@@ -8033,13 +8051,13 @@
     </row>
     <row r="160" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B160" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C160" s="27" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D160" s="25"/>
       <c r="E160" s="25" t="s">
@@ -8058,13 +8076,13 @@
     </row>
     <row r="161" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B161" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C161" s="27" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D161" s="25"/>
       <c r="E161" s="25" t="s">
@@ -8083,13 +8101,13 @@
     </row>
     <row r="162" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B162" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
       <c r="D162" s="25"/>
       <c r="E162" s="25" t="s">
@@ -8108,13 +8126,13 @@
     </row>
     <row r="163" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B163" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D163" s="25"/>
       <c r="E163" s="25" t="s">
@@ -8133,13 +8151,13 @@
     </row>
     <row r="164" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B164" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C164" s="27" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D164" s="25"/>
       <c r="E164" s="25" t="s">
@@ -8158,13 +8176,13 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B165" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C165" s="27" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D165" s="25"/>
       <c r="E165" s="25" t="s">
@@ -8183,13 +8201,13 @@
     </row>
     <row r="166" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B166" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C166" s="27" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D166" s="25"/>
       <c r="E166" s="25" t="s">
@@ -8208,13 +8226,13 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B167" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C167" s="27" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D167" s="25"/>
       <c r="E167" s="25" t="s">
@@ -8233,13 +8251,13 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B168" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C168" s="27" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D168" s="25"/>
       <c r="E168" s="25" t="s">
@@ -8258,13 +8276,13 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B169" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C169" s="27" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D169" s="25"/>
       <c r="E169" s="25" t="s">
@@ -8283,13 +8301,13 @@
     </row>
     <row r="170" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B170" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C170" s="27" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D170" s="25"/>
       <c r="E170" s="25" t="s">
@@ -8308,13 +8326,13 @@
     </row>
     <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B171" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C171" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D171" s="25"/>
       <c r="E171" s="25" t="s">
@@ -8333,13 +8351,13 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B172" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C172" s="27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D172" s="25"/>
       <c r="E172" s="25" t="s">
@@ -8358,13 +8376,13 @@
     </row>
     <row r="173" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A173" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B173" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C173" s="27" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D173" s="25"/>
       <c r="E173" s="25" t="s">
@@ -8383,13 +8401,13 @@
     </row>
     <row r="174" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B174" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C174" s="27" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D174" s="25"/>
       <c r="E174" s="25" t="s">
@@ -8408,13 +8426,13 @@
     </row>
     <row r="175" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B175" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C175" s="27" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D175" s="25"/>
       <c r="E175" s="25" t="s">
@@ -8433,13 +8451,13 @@
     </row>
     <row r="176" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B176" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C176" s="27" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D176" s="25"/>
       <c r="E176" s="25" t="s">
@@ -8458,13 +8476,13 @@
     </row>
     <row r="177" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B177" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C177" s="27" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D177" s="25"/>
       <c r="E177" s="25" t="s">
@@ -8483,13 +8501,13 @@
     </row>
     <row r="178" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B178" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C178" s="27" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D178" s="25"/>
       <c r="E178" s="25" t="s">
@@ -8508,13 +8526,13 @@
     </row>
     <row r="179" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B179" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C179" s="27" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D179" s="25"/>
       <c r="E179" s="25" t="s">
@@ -8533,13 +8551,13 @@
     </row>
     <row r="180" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A180" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B180" s="26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C180" s="27" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D180" s="25"/>
       <c r="E180" s="25" t="s">
@@ -8558,13 +8576,13 @@
     </row>
     <row r="181" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B181" s="26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C181" s="27" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D181" s="25"/>
       <c r="E181" s="25" t="s">
@@ -8583,13 +8601,13 @@
     </row>
     <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B182" s="26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C182" s="27" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D182" s="25"/>
       <c r="E182" s="25" t="s">
@@ -8608,13 +8626,13 @@
     </row>
     <row r="183" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C183" s="27" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D183" s="25"/>
       <c r="E183" s="25" t="s">
@@ -8633,13 +8651,13 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B184" s="26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C184" s="27" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D184" s="25"/>
       <c r="E184" s="25" t="s">
@@ -8658,13 +8676,13 @@
     </row>
     <row r="185" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B185" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C185" s="27" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D185" s="25"/>
       <c r="E185" s="25" t="s">
@@ -8683,13 +8701,13 @@
     </row>
     <row r="186" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B186" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C186" s="16" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="D186" s="25"/>
       <c r="E186" s="25" t="s">
@@ -8708,13 +8726,13 @@
     </row>
     <row r="187" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A187" s="25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B187" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C187" s="27" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D187" s="25"/>
       <c r="E187" s="25" t="s">
@@ -8733,13 +8751,13 @@
     </row>
     <row r="188" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B188" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C188" s="27" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D188" s="25"/>
       <c r="E188" s="25" t="s">
@@ -8758,13 +8776,13 @@
     </row>
     <row r="189" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B189" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C189" s="16" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25" t="s">
@@ -8783,13 +8801,13 @@
     </row>
     <row r="190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B190" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C190" s="27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D190" s="25"/>
       <c r="E190" s="25" t="s">
@@ -8808,13 +8826,13 @@
     </row>
     <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B191" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C191" s="27" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25" t="s">
@@ -8833,13 +8851,13 @@
     </row>
     <row r="192" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B192" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C192" s="27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D192" s="25"/>
       <c r="E192" s="25" t="s">
@@ -8858,13 +8876,13 @@
     </row>
     <row r="193" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B193" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C193" s="16" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D193" s="25"/>
       <c r="E193" s="25" t="s">
@@ -8883,13 +8901,13 @@
     </row>
     <row r="194" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A194" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B194" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C194" s="27" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D194" s="25"/>
       <c r="E194" s="25" t="s">
@@ -8908,13 +8926,13 @@
     </row>
     <row r="195" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B195" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C195" s="27" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D195" s="25"/>
       <c r="E195" s="25" t="s">
@@ -8933,13 +8951,13 @@
     </row>
     <row r="196" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B196" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C196" s="16" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="D196" s="25"/>
       <c r="E196" s="25" t="s">
@@ -8958,13 +8976,13 @@
     </row>
     <row r="197" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A197" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B197" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C197" s="27" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D197" s="25"/>
       <c r="E197" s="25" t="s">
@@ -8983,13 +9001,13 @@
     </row>
     <row r="198" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B198" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C198" s="27" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D198" s="25"/>
       <c r="E198" s="25" t="s">
@@ -9008,13 +9026,13 @@
     </row>
     <row r="199" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B199" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C199" s="27" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D199" s="25"/>
       <c r="E199" s="25" t="s">
@@ -9033,13 +9051,13 @@
     </row>
     <row r="200" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B200" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C200" s="27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D200" s="25"/>
       <c r="E200" s="25" t="s">
@@ -9058,13 +9076,13 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B201" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C201" s="27" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D201" s="25"/>
       <c r="E201" s="25" t="s">
@@ -9083,13 +9101,13 @@
     </row>
     <row r="202" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A202" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B202" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C202" s="27" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D202" s="25"/>
       <c r="E202" s="25" t="s">
@@ -9108,13 +9126,13 @@
     </row>
     <row r="203" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B203" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C203" s="27" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D203" s="25"/>
       <c r="E203" s="25" t="s">
@@ -9133,13 +9151,13 @@
     </row>
     <row r="204" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B204" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C204" s="16" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="D204" s="25"/>
       <c r="E204" s="25" t="s">
@@ -9158,13 +9176,13 @@
     </row>
     <row r="205" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B205" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C205" s="27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D205" s="25"/>
       <c r="E205" s="25" t="s">
@@ -9183,13 +9201,13 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B206" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C206" s="27" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D206" s="25"/>
       <c r="E206" s="25" t="s">
@@ -9208,13 +9226,13 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B207" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C207" s="16" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="D207" s="25"/>
       <c r="E207" s="25" t="s">
@@ -9233,13 +9251,13 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B208" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C208" s="27" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D208" s="25"/>
       <c r="E208" s="25" t="s">
@@ -9258,13 +9276,13 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B209" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C209" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D209" s="25"/>
       <c r="E209" s="25" t="s">
@@ -9283,13 +9301,13 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B210" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C210" s="27" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D210" s="25"/>
       <c r="E210" s="25" t="s">
@@ -9308,13 +9326,13 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B211" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C211" s="27" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D211" s="25"/>
       <c r="E211" s="25" t="s">
@@ -9333,13 +9351,13 @@
     </row>
     <row r="212" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B212" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C212" s="27" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D212" s="25"/>
       <c r="E212" s="25" t="s">
@@ -9358,13 +9376,13 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B213" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C213" s="27" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D213" s="25"/>
       <c r="E213" s="25" t="s">
@@ -9383,13 +9401,13 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B214" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C214" s="27" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D214" s="25"/>
       <c r="E214" s="25" t="s">
@@ -9408,13 +9426,13 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B215" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C215" s="27" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D215" s="25"/>
       <c r="E215" s="25" t="s">
@@ -9433,13 +9451,13 @@
     </row>
     <row r="216" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B216" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C216" s="27" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D216" s="25"/>
       <c r="E216" s="25" t="s">
@@ -9458,13 +9476,13 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B217" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C217" s="27" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D217" s="25"/>
       <c r="E217" s="25" t="s">
@@ -9483,13 +9501,13 @@
     </row>
     <row r="218" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B218" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C218" s="27" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D218" s="25"/>
       <c r="E218" s="25" t="s">
@@ -9508,13 +9526,13 @@
     </row>
     <row r="219" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B219" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C219" s="27" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D219" s="25"/>
       <c r="E219" s="25" t="s">
@@ -9533,13 +9551,13 @@
     </row>
     <row r="220" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B220" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C220" s="27" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D220" s="25"/>
       <c r="E220" s="25" t="s">
@@ -9558,13 +9576,13 @@
     </row>
     <row r="221" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B221" s="26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C221" s="27" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D221" s="25"/>
       <c r="E221" s="25" t="s">
@@ -9583,13 +9601,13 @@
     </row>
     <row r="222" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A222" s="25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B222" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C222" s="27" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D222" s="25"/>
       <c r="E222" s="25" t="s">
@@ -9608,13 +9626,13 @@
     </row>
     <row r="223" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B223" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C223" s="27" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D223" s="25"/>
       <c r="E223" s="25" t="s">
@@ -9633,13 +9651,13 @@
     </row>
     <row r="224" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="25" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B224" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C224" s="27" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D224" s="25"/>
       <c r="E224" s="25" t="s">
@@ -9658,13 +9676,13 @@
     </row>
     <row r="225" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B225" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C225" s="27" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D225" s="25"/>
       <c r="E225" s="25" t="s">
@@ -9683,13 +9701,13 @@
     </row>
     <row r="226" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A226" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B226" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C226" s="27" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D226" s="25"/>
       <c r="E226" s="25" t="s">
@@ -9708,13 +9726,13 @@
     </row>
     <row r="227" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B227" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C227" s="27" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D227" s="25"/>
       <c r="E227" s="25" t="s">
@@ -9733,13 +9751,13 @@
     </row>
     <row r="228" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B228" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C228" s="27" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D228" s="25"/>
       <c r="E228" s="25" t="s">
@@ -9758,13 +9776,13 @@
     </row>
     <row r="229" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B229" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C229" s="27" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D229" s="25"/>
       <c r="E229" s="25" t="s">
@@ -9783,13 +9801,13 @@
     </row>
     <row r="230" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B230" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C230" s="27" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D230" s="25"/>
       <c r="E230" s="25" t="s">
@@ -9808,13 +9826,13 @@
     </row>
     <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B231" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C231" s="27" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D231" s="25"/>
       <c r="E231" s="25" t="s">
@@ -9833,13 +9851,13 @@
     </row>
     <row r="232" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B232" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C232" s="27" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D232" s="25"/>
       <c r="E232" s="25" t="s">
@@ -9858,13 +9876,13 @@
     </row>
     <row r="233" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B233" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C233" s="27" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D233" s="25"/>
       <c r="E233" s="25" t="s">
@@ -9883,13 +9901,13 @@
     </row>
     <row r="234" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B234" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C234" s="27" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D234" s="25"/>
       <c r="E234" s="25" t="s">
@@ -9908,13 +9926,13 @@
     </row>
     <row r="235" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A235" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B235" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C235" s="27" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D235" s="25"/>
       <c r="E235" s="25" t="s">
@@ -9933,13 +9951,13 @@
     </row>
     <row r="236" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A236" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B236" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C236" s="27" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D236" s="25"/>
       <c r="E236" s="25" t="s">
@@ -9958,13 +9976,13 @@
     </row>
     <row r="237" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A237" s="25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B237" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C237" s="27" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D237" s="25"/>
       <c r="E237" s="25" t="s">
@@ -9983,13 +10001,13 @@
     </row>
     <row r="238" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B238" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C238" s="27" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D238" s="25"/>
       <c r="E238" s="25" t="s">
@@ -10008,16 +10026,16 @@
     </row>
     <row r="239" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B239" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C239" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D239" s="25" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E239" s="25" t="s">
         <v>22</v>
@@ -10032,21 +10050,21 @@
         <v>21</v>
       </c>
       <c r="I239" s="27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="240" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A240" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B240" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C240" s="27" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D240" s="25" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E240" s="25" t="s">
         <v>22</v>
@@ -10061,21 +10079,21 @@
         <v>20</v>
       </c>
       <c r="I240" s="27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="241" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="A241" s="25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B241" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C241" s="27" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D241" s="25" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E241" s="25" t="s">
         <v>22</v>
@@ -10093,16 +10111,16 @@
     </row>
     <row r="242" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" s="25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B242" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C242" s="27" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D242" s="25" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E242" s="25" t="s">
         <v>22</v>
@@ -10120,16 +10138,16 @@
     </row>
     <row r="243" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" s="25" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B243" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C243" s="27" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D243" s="25" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E243" s="25" t="s">
         <v>22</v>
@@ -10147,13 +10165,13 @@
     </row>
     <row r="244" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A244" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B244" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C244" s="27" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D244" s="25"/>
       <c r="E244" s="25" t="s">
@@ -10172,13 +10190,13 @@
     </row>
     <row r="245" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A245" s="25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B245" s="26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C245" s="28" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D245" s="25"/>
       <c r="E245" s="25" t="s">
@@ -10197,13 +10215,13 @@
     </row>
     <row r="246" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A246" s="25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B246" s="26" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C246" s="28" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D246" s="25"/>
       <c r="E246" s="25" t="s">
@@ -10222,13 +10240,13 @@
     </row>
     <row r="247" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B247" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C247" s="27" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D247" s="25"/>
       <c r="E247" s="25" t="s">
@@ -10247,13 +10265,13 @@
     </row>
     <row r="248" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A248" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B248" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C248" s="27" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D248" s="25"/>
       <c r="E248" s="25" t="s">
@@ -10272,13 +10290,13 @@
     </row>
     <row r="249" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B249" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C249" s="27" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D249" s="25"/>
       <c r="E249" s="25" t="s">
@@ -10297,13 +10315,13 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B250" s="26" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C250" s="27" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D250" s="25"/>
       <c r="E250" s="25" t="s">
@@ -10322,13 +10340,13 @@
     </row>
     <row r="251" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A251" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B251" s="26" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C251" s="27" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D251" s="25"/>
       <c r="E251" s="25" t="s">
@@ -10347,13 +10365,13 @@
     </row>
     <row r="252" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A252" s="25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B252" s="26" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C252" s="27" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D252" s="25"/>
       <c r="E252" s="25" t="s">
@@ -10372,13 +10390,13 @@
     </row>
     <row r="253" spans="1:9" ht="360" x14ac:dyDescent="0.25">
       <c r="A253" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B253" s="26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C253" s="27" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D253" s="25"/>
       <c r="E253" s="25" t="s">
@@ -10516,112 +10534,11 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B244:B255 B10:B243" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B244:B255 B10:B16 B18:B243 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all/>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/office/internal/2005/internalDocumentation" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type" ma:readOnly="true"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="lastPrinted" minOccurs="0" maxOccurs="1" type="xsd:dateTime"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change MS-OXWSBTRF_RequirementSpecification.xlsx,MS-OXWSBTRF_RequirementSpecification.xml,[MS-OXWSBTRF].md according to v20181001
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSBTRF/MS-OXWSBTRF_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSBTRF/MS-OXWSBTRF_RequirementSpecification.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF50B3D-1067-4A36-B06B-6E250BB2AC37}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -20,15 +21,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmp517C" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmp517C" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-penj\AppData\Local\Temp\tmp517C.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="567">
   <si>
     <t>Req ID</t>
   </si>
@@ -1115,22 +1116,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>2.2.3.22</t>
-  </si>
-  <si>
-    <t>2.2.3.23</t>
-  </si>
-  <si>
-    <t>2.2.4.10</t>
-  </si>
-  <si>
     <t>2.2.4.16</t>
-  </si>
-  <si>
-    <t>2.2.4.57</t>
-  </si>
-  <si>
-    <t>2.2.5.10</t>
   </si>
   <si>
     <t>[In Messages]In the following sections, the schema definition might differ from the processing rules imposed by the protocol.</t>
@@ -1873,12 +1859,6 @@
   </si>
   <si>
     <t>[In CreateActionType Simple Type][UpdateOrCreate][If the target item is not in the original folder specified by the &lt;ParentFolderId&gt; element in the UploadItemType complex type]The &lt;ItemId&gt; element that is returned in the UploadItemsResponseMessageType complex type, as specified in section 3.1.4.2.3.2, MUST contain the new item identifier.</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms SHOULD or SHOULD NOT implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Unless otherwise specified, the term MAY implies that the product does not follow the prescription.</t>
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does use secure communications via HTTPS, as defined in [RFC2818]. (Exchange Server 2010 and above follow this behavior.)</t>
@@ -2043,182 +2023,6 @@
   </si>
   <si>
     <t>Verified by derived requirement: MS-OXWSBTRF_R2111.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In m:ArrayOfResponseMessagesType Complex Type] The type [ArrayOfResponseMessagesType] is defined as follow:
-&lt;xs:complexType name="ArrayOfResponseMessagesType"&gt;
-  &lt;xs:choice
-    maxOccurs="unbounded"
-  &gt;
-    &lt;xs:element name="CreateItemResponseMessage"
-      type="m:ItemInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="DeleteItemResponseMessage"
-      type="m:ResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetItemResponseMessage"
-      type="m:ItemInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="UpdateItemResponseMessage"
-      type="m:UpdateItemResponseMessageType"
-     /&gt;
-    &lt;xs:element name="UpdateItemInRecoverableItemsResponseMessage" 
-     type="m:UpdateItemInRecoverableItemsResponseMessageType"/&gt;
-    &lt;xs:element name="SendItemResponseMessage"
-      type="m:ResponseMessageType"
-     /&gt;
-    &lt;xs:element name="DeleteFolderResponseMessage"
-      type="m:ResponseMessageType"
-     /&gt;
-    &lt;xs:element name="EmptyFolderResponseMessage"
-      type="m:ResponseMessageType"
-     /&gt;
-    &lt;xs:element name="CreateFolderResponseMessage"
-      type="m:FolderInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetFolderResponseMessage"
-      type="m:FolderInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="FindFolderResponseMessage"
-      type="m:FindFolderResponseMessageType"
-     /&gt;
-    &lt;xs:element name="UpdateFolderResponseMessage"
-      type="m:FolderInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="MoveFolderResponseMessage"
-      type="m:FolderInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="CopyFolderResponseMessage"
-      type="m:FolderInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="CreateFolderPathResponseMessage" 
-     type="m:FolderInfoResponseMessageType"
-    /&gt;
-    &lt;xs:element name="CreateAttachmentResponseMessage"
-      type="m:AttachmentInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="DeleteAttachmentResponseMessage"
-      type="m:DeleteAttachmentResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetAttachmentResponseMessage"
-      type="m:AttachmentInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="UploadItemsResponseMessage"
-      type="m:UploadItemsResponseMessageType"
-     /&gt;
-    &lt;xs:element name="ExportItemsResponseMessage"
-      type="m:ExportItemsResponseMessageType"
-     /&gt;
-    &lt;xs:element name="MarkAllItemsAsReadResponseMessage" 
-       type="m:ResponseMessageType"/&gt;
-    &lt;xs:element name="GetClientAccessTokenResponseMessage" 
-       type="m:GetClientAccessTokenResponseMessageType"/&gt;
-    &lt;xs:element name="GetAppManifestsResponseMessage" type="m:ResponseMessageType"/&gt;
-    &lt;xs:element name="GetClientExtensionResponseMessage" 
-       type="m:ResponseMessageType"/&gt;
-    &lt;xs:element name="SetClientExtensionResponseMessage" 
-       type="m:ResponseMessageType"/&gt;
-    &lt;xs:element name="FindItemResponseMessage"
-      type="m:FindItemResponseMessageType"
-     /&gt;
-    &lt;xs:element name="MoveItemResponseMessage"
-      type="m:ItemInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="ArchiveItemResponseMessage" type="m:ItemInfoResponseMessageType"/&gt;
-    &lt;xs:element name="CopyItemResponseMessage"
-      type="m:ItemInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="ResolveNamesResponseMessage"
-      type="m:ResolveNamesResponseMessageType"
-     /&gt;
-    &lt;xs:element name="ExpandDLResponseMessage"
-      type="m:ExpandDLResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetServerTimeZonesResponseMessage"
-      type="m:GetServerTimeZonesResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetEventsResponseMessage"
-      type="m:GetEventsResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetStreamingEventsResponseMessage"
-      type="m:GetStreamingEventsResponseMessageType"
-     /&gt;
-    &lt;xs:element name="SubscribeResponseMessage"
-      type="m:SubscribeResponseMessageType"
-     /&gt;
-    &lt;xs:element name="UnsubscribeResponseMessage"
-      type="m:ResponseMessageType"
-     /&gt;
-    &lt;xs:element name="SendNotificationResponseMessage"
-      type="m:SendNotificationResponseMessageType"
-     /&gt;
-    &lt;xs:element name="SyncFolderHierarchyResponseMessage"
-      type="m:SyncFolderHierarchyResponseMessageType"
-     /&gt;
-    &lt;xs:element name="SyncFolderItemsResponseMessage"
-      type="m:SyncFolderItemsResponseMessageType"
-     /&gt;
-    &lt;xs:element name="CreateManagedFolderResponseMessage"
-      type="m:FolderInfoResponseMessageType"
-     /&gt;
-    &lt;xs:element name="ConvertIdResponseMessage"
-      type="m:ConvertIdResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetSharingMetadataResponseMessage"
-      type="m:GetSharingMetadataResponseMessageType"
-     /&gt;
-    &lt;xs:element name="RefreshSharingFolderResponseMessage"
-      type="m:RefreshSharingFolderResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetSharingFolderResponseMessage"
-      type="m:GetSharingFolderResponseMessageType"
-     /&gt;
-    &lt;xs:element name="CreateUserConfigurationResponseMessage"
-      type="m:ResponseMessageType"
-     /&gt;
-    &lt;xs:element name="DeleteUserConfigurationResponseMessage"
-      type="m:ResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetUserConfigurationResponseMessage"
-      type="m:GetUserConfigurationResponseMessageType"
-     /&gt;
-    &lt;xs:element name="UpdateUserConfigurationResponseMessage"
-      type="m:ResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetRoomListsResponse"
-      type="m:GetRoomListsResponseMessageType"
-     /&gt;
-    &lt;xs:element name="GetRoomsResponse"
-      type="m:GetRoomsResponseMessageType"
-     /&gt;
-      &lt;xs:element name="GetRemindersResponse" 
-       type="m:GetRemindersResponseMessageType"/&gt;
-      &lt;xs:element name="PerformReminderActionResponse" 
-       type="m:PerformReminderActionResponseMessageType"/&gt;
-    &lt;xs:element name="ApplyConversationActionResponseMessage"
-      type="m:ResponseMessageType"
-     /&gt;
-    &lt;xs:element name="FindMailboxStatisticsByKeywordsResponseMessage" type="m:FindMailboxStatisticsByKeywordsResponseMessageType"/&gt;
-    &lt;xs:element name="GetSearchableMailboxesResponseMessage" type="m:GetSearchableMailboxesResponseMessageType"/&gt;
-    &lt;xs:element name="SearchMailboxesResponseMessage" type="m:SearchMailboxesResponseMessageType"/&gt;
-    &lt;xs:element name="GetDiscoverySearchConfigurationResponseMessage" type="m:GetDiscoverySearchConfigurationResponseMessageType"/&gt;
-    &lt;xs:element name="GetHoldOnMailboxesResponseMessage" type="m:GetHoldOnMailboxesResponseMessageType"/&gt;
-    &lt;xs:element name="SetHoldOnMailboxesResponseMessage" type="m:SetHoldOnMailboxesResponseMessageType"/&gt;
-      &lt;xs:element name="GetNonIndexableItemStatisticsResponseMessage" type="m:GetNonIndexableItemStatisticsResponseMessageType"/&gt;
-      &lt;!-- GetNonIndexableItemDetails response --&gt;
-      &lt;xs:element name="GetNonIndexableItemDetailsResponseMessage" type="m:GetNonIndexableItemDetailsResponseMessageType"/&gt;
-      &lt;!-- GetUserHoldSettings response --&gt;
-    &lt;xs:element name="FindPeopleResponseMessage" type="m:FindPeopleResponseMessageType"/&gt;
-    &lt;xs:element name="GetPasswordExpirationDateResponse" type="m:GetPasswordExpirationDateResponseMessageType"
-    /&gt;
-      &lt;xs:element name="GetPersonaResponseMessage" type="m:GetPersonaResponseMessageType"/&gt;
-      &lt;xs:element name="GetConversationItemsResponseMessage" type="m:GetConversationItemsResponseMessageType"/&gt;
-      &lt;xs:element name="GetUserRetentionPolicyTagsResponseMessage" type="m:GetUserRetentionPolicyTagsResponseMessageType"/&gt;
-      &lt;xs:element name="GetUserPhotoResponseMessage" type="m:GetUserPhotoResponseMessageType"/&gt;
-      &lt;xs:element name="MarkAsJunkResponseMessage" type="m:MarkAsJunkResponseMessageType"/&gt;
-  &lt;/xs:choice&gt;
-&lt;/xs:complexType&gt;
-</t>
   </si>
   <si>
     <t xml:space="preserve">[In m:ResponseCodeType Simple Type] The type [ResponseCodeType] is defined as follow:
@@ -2698,18 +2502,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In tns:ExportItemsSoapIn Message]The type of MailboxCulture is t:MailboxCulture ([MS-OXWSCDATA] section 2.2.3.7).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In tns:ExportItemsSoapIn Message]The type of RequestVersion is t:RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.11).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In tns:ExportItemsSoapIn Message]The part ManagementRole with Element/type t:ManagementRole ([MS-OXWSCDATA] section 2.2.3.8): specifies the SOAP header that identifies the caller's role. &lt;2&gt; .</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In tns:ExportItemsSoapOut Message][If the request is unsuccessful]The ResponseCode element of the ExportItemsResponseMessage element is set to a value of the ResponseCodeType simple type, as specified in [MS-OXWSCDATA] section 2.2.5.24.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2733,20 +2525,6 @@
   <si>
     <t>[In tns:UploadItemsSoapIn Message]The Element/type of Impersonation
  is ExchangeImpersonation ([MS-OXWSCDATA] section 2.2.3.3).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In tns:UploadItemsSoapIn Message]The Element/type of MailboxCulture is
-MailboxCulture ([MS-OXWSCDATA] section 2.2.3.7).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In tns:UploadItemsSoapIn Message]The Element/type of RequestVersion is
-RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.11).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In tns:UploadItemsSoapOut Message]The Element/type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.3.12).</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2864,10 +2642,6 @@
     </r>
   </si>
   <si>
-    <t>[In tns:ExportItemsSoapOut Message]The type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.3.12).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In m:ExportItemsResponseMessageType Complex Type]The type of ItemId is t:ItemIdType ([MS-OXWSCORE] section 2.2.4.25).</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2878,12 +2652,249 @@
   <si>
     <t>[In tns:UploadItemsSoapOut Message][If the request UploadItems request is unsuccessful]The ResponseCode element of the UploadItemsResponseMessage element is set to a value of the ResponseCodeType simple type, as specified in [MS-OXWSCDATA] section 2.2.5.24.</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapIn Message]The type of MailboxCulture is t:MailboxCulture ([MS-OXWSCDATA] section 2.2.3.6).</t>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapIn Message]The type of RequestVersion is t:RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.9).</t>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapIn Message]The part ManagementRole with Element/type t:ManagementRole ([MS-OXWSCDATA] section 2.2.3.7): specifies the SOAP header that identifies the caller's role. &lt;2&gt; .</t>
+  </si>
+  <si>
+    <t>[In tns:ExportItemsSoapOut Message]The type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.3.10).</t>
+  </si>
+  <si>
+    <t>[In tns:UploadItemsSoapIn Message]The Element/type of MailboxCulture is
+MailboxCulture ([MS-OXWSCDATA] section 2.2.3.6).</t>
+  </si>
+  <si>
+    <t>[In tns:UploadItemsSoapIn Message]The Element/type of RequestVersion is
+RequestServerVersion ([MS-OXWSCDATA] section 2.2.3.9).</t>
+  </si>
+  <si>
+    <t>[In tns:UploadItemsSoapOut Message]The Element/type of ServerVersion is ServerVersion ([MS-OXWSCDATA] section 2.2.3.10).</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms SHOULD or SHOULD NOT implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Unless otherwise specified, the term MAY implies that the product does not follow the prescription.</t>
+  </si>
+  <si>
+    <t>2.2.5.23</t>
+  </si>
+  <si>
+    <t>2.2.5.24</t>
+  </si>
+  <si>
+    <t>2.2.4.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	&lt;xs:complexType name="ArrayOfResponseMessagesType"&gt;
+	  &lt;xs:choice
+	    maxOccurs="unbounded"
+	  &gt;
+	    &lt;xs:element name="CreateItemResponseMessage"
+	      type="m:ItemInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="DeleteItemResponseMessage"
+	      type=" m:DeleteItemResponseMessageType "
+	     /&gt;
+	    &lt;xs:element name="GetItemResponseMessage"
+	      type="m:ItemInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="UpdateItemResponseMessage"
+	      type="m:UpdateItemResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="UpdateItemInRecoverableItemsResponseMessage" 
+	     type="m:UpdateItemInRecoverableItemsResponseMessageType"/&gt;
+	    &lt;xs:element name="SendItemResponseMessage"
+	      type="m:ResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="DeleteFolderResponseMessage"
+	      type="m:ResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="EmptyFolderResponseMessage"
+	      type="m:ResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="CreateFolderResponseMessage"
+	      type="m:FolderInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetFolderResponseMessage"
+	      type="m:FolderInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="FindFolderResponseMessage"
+	      type="m:FindFolderResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="UpdateFolderResponseMessage"
+	      type="m:FolderInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="MoveFolderResponseMessage"
+	      type="m:FolderInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="CopyFolderResponseMessage"
+	      type="m:FolderInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="CreateFolderPathResponseMessage" 
+	     type="m:FolderInfoResponseMessageType"
+	    /&gt;
+	    &lt;xs:element name="CreateAttachmentResponseMessage"
+	      type="m:AttachmentInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="DeleteAttachmentResponseMessage"
+	      type="m:DeleteAttachmentResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetAttachmentResponseMessage"
+	      type="m:AttachmentInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="UploadItemsResponseMessage"
+	      type="m:UploadItemsResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="ExportItemsResponseMessage"
+	      type="m:ExportItemsResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="MarkAllItemsAsReadResponseMessage" 
+	       type="m:ResponseMessageType"/&gt;
+	    &lt;xs:element name="GetClientAccessTokenResponseMessage" 
+	       type="m:GetClientAccessTokenResponseMessageType"/&gt;
+	    &lt;xs:element name="GetAppManifestsResponseMessage" type="m:ResponseMessageType"/&gt;
+	    &lt;xs:element name="GetClientExtensionResponseMessage" 
+	       type="m:ResponseMessageType"/&gt;
+	    &lt;xs:element name="SetClientExtensionResponseMessage" 
+	       type="m:ResponseMessageType"/&gt;
+	    &lt;xs:element name="GetOMEConfigurationResponseMessage" type="m:ResponseMessageType"/&gt;
+		&lt;xs:element name="SetOMEConfigurationResponseMessage" type="m:ResponseMessageType"/&gt;
+	    &lt;xs:element name="FindItemResponseMessage"
+	      type="m:FindItemResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="MoveItemResponseMessage"
+	      type="m:ItemInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="ArchiveItemResponseMessage" type="m:ItemInfoResponseMessageType"/&gt;
+	    &lt;xs:element name="CopyItemResponseMessage"
+	      type="m:ItemInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="ResolveNamesResponseMessage"
+	      type="m:ResolveNamesResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="ExpandDLResponseMessage"
+	      type="m:ExpandDLResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetServerTimeZonesResponseMessage"
+	      type="m:GetServerTimeZonesResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetEventsResponseMessage"
+	      type="m:GetEventsResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetStreamingEventsResponseMessage"
+	      type="m:GetStreamingEventsResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="SubscribeResponseMessage"
+	      type="m:SubscribeResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="UnsubscribeResponseMessage"
+	      type="m:ResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetChannelEventsResponseMessage"
+	      type="m:GetChannelEventsResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="ChannelSubscribeResponseMessage" 
+	      type="m:ChannelSubscribeResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="ChannelUnsubscribeResponseMessage" 
+	      type="m:ResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="SendNotificationResponseMessage"
+	      type="m:SendNotificationResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="SyncFolderHierarchyResponseMessage"
+	      type="m:SyncFolderHierarchyResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="SyncFolderItemsResponseMessage"
+	      type="m:SyncFolderItemsResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="CreateManagedFolderResponseMessage"
+	      type="m:FolderInfoResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="ConvertIdResponseMessage"
+	      type="m:ConvertIdResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetSharingMetadataResponseMessage"
+	      type="m:GetSharingMetadataResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="RefreshSharingFolderResponseMessage"
+	      type="m:RefreshSharingFolderResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetSharingFolderResponseMessage"
+	      type="m:GetSharingFolderResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="CreateUserConfigurationResponseMessage"
+	      type="m:ResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="DeleteUserConfigurationResponseMessage"
+	      type="m:ResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetUserConfigurationResponseMessage"
+	      type="m:GetUserConfigurationResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="UpdateUserConfigurationResponseMessage"
+	      type="m:ResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetRoomListsResponse"
+	      type="m:GetRoomListsResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="GetRoomsResponse"
+	      type="m:GetRoomsResponseMessageType"   
+	     /&gt;
+	    &lt;xs:element name="GetRemindersResponse" 
+	       type="m:GetRemindersResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="PerformReminderActionResponse" 
+	       type="m:PerformReminderActionResponseMessageType"
+	     /&gt;
+	    &lt;xs:element name="ApplyConversationActionResponseMessage"
+	      type="m:ApplyConversationActionResponseMessageType"/&gt;
+	    &lt;xs:element name="FindMailboxStatisticsByKeywordsResponseMessage" type="m:FindMailboxStatisticsByKeywordsResponseMessageType"/&gt;
+	    &lt;xs:element name="GetSearchableMailboxesResponseMessage" type="m:GetSearchableMailboxesResponseMessageType"/&gt;
+	    &lt;xs:element name="SearchMailboxesResponseMessage" type="m:SearchMailboxesResponseMessageType"/&gt;
+	    &lt;xs:element name="GetDiscoverySearchConfigurationResponseMessage" type="m:GetDiscoverySearchConfigurationResponseMessageType"/&gt;
+	    &lt;xs:element name="GetHoldOnMailboxesResponseMessage" type="m:GetHoldOnMailboxesResponseMessageType"/&gt;
+	    &lt;xs:element name="SetHoldOnMailboxesResponseMessage" type="m:SetHoldOnMailboxesResponseMessageType"/&gt;
+	      &lt;xs:element name="GetNonIndexableItemStatisticsResponseMessage" type="m:GetNonIndexableItemStatisticsResponseMessageType"/&gt;
+	      &lt;!-- GetNonIndexableItemDetails response --&gt;
+	      &lt;xs:element name="GetNonIndexableItemDetailsResponseMessage" type="m:GetNonIndexableItemDetailsResponseMessageType"/&gt;
+	    &lt;xs:element name="FindPeopleResponseMessage" type="m:FindPeopleResponseMessageType"/&gt;
+	    &lt;xs:element name="GetPasswordExpirationDateResponse" type="m:GetPasswordExpirationDateResponseMessageType"
+	    /&gt;
+	      &lt;xs:element name="GetPersonaResponseMessage" type="m:GetPersonaResponseMessageType"/&gt;
+	      &lt;xs:element name="GetConversationItemsResponseMessage" type="m:GetConversationItemsResponseMessageType"/&gt;
+	      &lt;xs:element name="GetUserRetentionPolicyTagsResponseMessage" type="m:GetUserRetentionPolicyTagsResponseMessageType"/&gt;
+	      &lt;xs:element name="GetUserPhotoResponseMessage" type="m:GetUserPhotoResponseMessageType"/&gt;
+	      &lt;xs:element name="MarkAsJunkResponseMessage" type="m:MarkAsJunkResponseMessageType"/&gt;
+	      &lt;xs:element name="UpdateMailboxAssociationResponseMessage" type="m:ResponseMessageType"/&gt;
+	      &lt;xs:element name="UpdateGroupMailboxResponseMessage" type="m:ResponseMessageType"/&gt;
+	      &lt;xs:element name="PostModernGroupItemResponseMessage" type="m:ResponseMessageType"/&gt;
+	      &lt;xs:element name="LikeItemResponseMessage" type="m:ResponseMessageType"/&gt;
+	      &lt;xs:element name="GetUnifiedGroupUnseenDataResponseMessage" type="m:GetUnifiedGroupUnseenDataResponseMessageType"/&gt;
+	  &lt;/xs:choice&gt;
+	&lt;/xs:complexType&gt;</t>
+  </si>
+  <si>
+    <t>2.2.4.18</t>
+  </si>
+  <si>
+    <t>2.2.4.67</t>
+  </si>
+  <si>
+    <t>2.2.3.10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -3852,34 +3863,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I253" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
-  <autoFilter ref="A19:I253"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I253" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
+  <autoFilter ref="A19:I253" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="12">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -3888,12 +3899,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3975,6 +3986,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4010,6 +4038,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4185,11 +4230,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -4208,7 +4255,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -4220,7 +4267,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4238,14 +4285,14 @@
         <v>25</v>
       </c>
       <c r="C3" s="36">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="35" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="37">
-        <v>42261</v>
+        <v>43374</v>
       </c>
       <c r="G3" s="38"/>
       <c r="H3" s="4"/>
@@ -4324,7 +4371,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="C8" s="55"/>
       <c r="D8" s="55"/>
@@ -4375,7 +4422,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="C11" s="61"/>
       <c r="D11" s="47"/>
@@ -4485,7 +4532,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="64" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="C17" s="65"/>
       <c r="D17" s="65"/>
@@ -4502,7 +4549,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
@@ -4553,7 +4600,7 @@
         <v>273</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18" t="s">
@@ -4578,7 +4625,7 @@
         <v>273</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18" t="s">
@@ -4603,7 +4650,7 @@
         <v>274</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18" t="s">
@@ -4628,7 +4675,7 @@
         <v>274</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18" t="s">
@@ -4653,7 +4700,7 @@
         <v>274</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18" t="s">
@@ -4678,7 +4725,7 @@
         <v>274</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18" t="s">
@@ -4703,7 +4750,7 @@
         <v>274</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18" t="s">
@@ -4728,7 +4775,7 @@
         <v>275</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18" t="s">
@@ -4753,7 +4800,7 @@
         <v>275</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="18" t="s">
@@ -4778,7 +4825,7 @@
         <v>275</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18" t="s">
@@ -4803,7 +4850,7 @@
         <v>275</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18" t="s">
@@ -4819,7 +4866,7 @@
         <v>17</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="19" customFormat="1" ht="30">
@@ -4830,7 +4877,7 @@
         <v>276</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18" t="s">
@@ -4855,7 +4902,7 @@
         <v>276</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18" t="s">
@@ -4880,7 +4927,7 @@
         <v>277</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18" t="s">
@@ -4905,7 +4952,7 @@
         <v>277</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="25" t="s">
@@ -4930,7 +4977,7 @@
         <v>277</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D35" s="25"/>
       <c r="E35" s="25" t="s">
@@ -4955,7 +5002,7 @@
         <v>277</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D36" s="25"/>
       <c r="E36" s="25" t="s">
@@ -4980,7 +5027,7 @@
         <v>277</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D37" s="25"/>
       <c r="E37" s="25" t="s">
@@ -5005,7 +5052,7 @@
         <v>277</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="25" t="s">
@@ -5030,7 +5077,7 @@
         <v>277</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="25" t="s">
@@ -5055,7 +5102,7 @@
         <v>277</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="25" t="s">
@@ -5080,7 +5127,7 @@
         <v>277</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D41" s="25"/>
       <c r="E41" s="25" t="s">
@@ -5105,7 +5152,7 @@
         <v>277</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D42" s="25"/>
       <c r="E42" s="25" t="s">
@@ -5130,7 +5177,7 @@
         <v>278</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D43" s="25"/>
       <c r="E43" s="25" t="s">
@@ -5155,7 +5202,7 @@
         <v>279</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D44" s="25"/>
       <c r="E44" s="25" t="s">
@@ -5180,7 +5227,7 @@
         <v>280</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D45" s="25"/>
       <c r="E45" s="25" t="s">
@@ -5205,7 +5252,7 @@
         <v>281</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D46" s="25"/>
       <c r="E46" s="25" t="s">
@@ -5230,7 +5277,7 @@
         <v>282</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D47" s="25"/>
       <c r="E47" s="25" t="s">
@@ -5255,7 +5302,7 @@
         <v>283</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D48" s="25"/>
       <c r="E48" s="25" t="s">
@@ -5280,7 +5327,7 @@
         <v>284</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D49" s="25"/>
       <c r="E49" s="25" t="s">
@@ -5305,7 +5352,7 @@
         <v>285</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D50" s="25"/>
       <c r="E50" s="25" t="s">
@@ -5330,7 +5377,7 @@
         <v>285</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="25" t="s">
@@ -5355,7 +5402,7 @@
         <v>285</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="D52" s="25"/>
       <c r="E52" s="25" t="s">
@@ -5380,7 +5427,7 @@
         <v>286</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="D53" s="25"/>
       <c r="E53" s="25" t="s">
@@ -5405,7 +5452,7 @@
         <v>286</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D54" s="25"/>
       <c r="E54" s="25" t="s">
@@ -5430,7 +5477,7 @@
         <v>287</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D55" s="25"/>
       <c r="E55" s="25" t="s">
@@ -5455,7 +5502,7 @@
         <v>287</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D56" s="25"/>
       <c r="E56" s="25" t="s">
@@ -5480,7 +5527,7 @@
         <v>287</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D57" s="25"/>
       <c r="E57" s="25" t="s">
@@ -5505,7 +5552,7 @@
         <v>287</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D58" s="25"/>
       <c r="E58" s="25" t="s">
@@ -5530,7 +5577,7 @@
         <v>31</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D59" s="25"/>
       <c r="E59" s="25" t="s">
@@ -5555,7 +5602,7 @@
         <v>31</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="D60" s="25"/>
       <c r="E60" s="25" t="s">
@@ -5580,7 +5627,7 @@
         <v>31</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D61" s="25"/>
       <c r="E61" s="25" t="s">
@@ -5596,7 +5643,7 @@
         <v>17</v>
       </c>
       <c r="I61" s="27" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="30">
@@ -5607,7 +5654,7 @@
         <v>288</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D62" s="25"/>
       <c r="E62" s="25" t="s">
@@ -5632,7 +5679,7 @@
         <v>288</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="D63" s="25"/>
       <c r="E63" s="25" t="s">
@@ -5657,7 +5704,7 @@
         <v>288</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="D64" s="25"/>
       <c r="E64" s="25" t="s">
@@ -5682,7 +5729,7 @@
         <v>289</v>
       </c>
       <c r="C65" s="27" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D65" s="25"/>
       <c r="E65" s="25" t="s">
@@ -5707,7 +5754,7 @@
         <v>289</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D66" s="25"/>
       <c r="E66" s="25" t="s">
@@ -5732,7 +5779,7 @@
         <v>289</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D67" s="25"/>
       <c r="E67" s="25" t="s">
@@ -5757,7 +5804,7 @@
         <v>289</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25" t="s">
@@ -5782,7 +5829,7 @@
         <v>289</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D69" s="25"/>
       <c r="E69" s="25" t="s">
@@ -5807,7 +5854,7 @@
         <v>289</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D70" s="25"/>
       <c r="E70" s="25" t="s">
@@ -5832,7 +5879,7 @@
         <v>289</v>
       </c>
       <c r="C71" s="27" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D71" s="25"/>
       <c r="E71" s="25" t="s">
@@ -5857,7 +5904,7 @@
         <v>289</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="D72" s="25"/>
       <c r="E72" s="25" t="s">
@@ -5882,7 +5929,7 @@
         <v>289</v>
       </c>
       <c r="C73" s="27" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D73" s="25"/>
       <c r="E73" s="25" t="s">
@@ -5907,7 +5954,7 @@
         <v>289</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D74" s="25"/>
       <c r="E74" s="25" t="s">
@@ -5932,7 +5979,7 @@
         <v>289</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="D75" s="25"/>
       <c r="E75" s="25" t="s">
@@ -5957,7 +6004,7 @@
         <v>289</v>
       </c>
       <c r="C76" s="27" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D76" s="25"/>
       <c r="E76" s="25" t="s">
@@ -5982,7 +6029,7 @@
         <v>289</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="D77" s="25"/>
       <c r="E77" s="25" t="s">
@@ -6007,7 +6054,7 @@
         <v>289</v>
       </c>
       <c r="C78" s="27" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D78" s="25"/>
       <c r="E78" s="25" t="s">
@@ -6032,7 +6079,7 @@
         <v>289</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
       <c r="D79" s="25"/>
       <c r="E79" s="25" t="s">
@@ -6057,7 +6104,7 @@
         <v>290</v>
       </c>
       <c r="C80" s="27" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D80" s="25"/>
       <c r="E80" s="25" t="s">
@@ -6082,7 +6129,7 @@
         <v>290</v>
       </c>
       <c r="C81" s="27" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D81" s="25"/>
       <c r="E81" s="25" t="s">
@@ -6107,7 +6154,7 @@
         <v>290</v>
       </c>
       <c r="C82" s="27" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D82" s="25"/>
       <c r="E82" s="25" t="s">
@@ -6132,7 +6179,7 @@
         <v>290</v>
       </c>
       <c r="C83" s="27" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D83" s="25"/>
       <c r="E83" s="25" t="s">
@@ -6157,7 +6204,7 @@
         <v>290</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="D84" s="25"/>
       <c r="E84" s="25" t="s">
@@ -6182,7 +6229,7 @@
         <v>290</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="D85" s="25"/>
       <c r="E85" s="25" t="s">
@@ -6207,7 +6254,7 @@
         <v>290</v>
       </c>
       <c r="C86" s="27" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D86" s="25"/>
       <c r="E86" s="25" t="s">
@@ -6232,7 +6279,7 @@
         <v>290</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D87" s="25"/>
       <c r="E87" s="25" t="s">
@@ -6257,7 +6304,7 @@
         <v>290</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D88" s="25"/>
       <c r="E88" s="25" t="s">
@@ -6282,7 +6329,7 @@
         <v>290</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D89" s="25"/>
       <c r="E89" s="25" t="s">
@@ -6307,7 +6354,7 @@
         <v>290</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>547</v>
+        <v>536</v>
       </c>
       <c r="D90" s="25"/>
       <c r="E90" s="25" t="s">
@@ -6332,7 +6379,7 @@
         <v>291</v>
       </c>
       <c r="C91" s="27" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D91" s="25"/>
       <c r="E91" s="25" t="s">
@@ -6357,7 +6404,7 @@
         <v>291</v>
       </c>
       <c r="C92" s="27" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D92" s="25"/>
       <c r="E92" s="25" t="s">
@@ -6382,7 +6429,7 @@
         <v>291</v>
       </c>
       <c r="C93" s="27" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D93" s="25"/>
       <c r="E93" s="25" t="s">
@@ -6407,7 +6454,7 @@
         <v>292</v>
       </c>
       <c r="C94" s="27" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D94" s="25"/>
       <c r="E94" s="25" t="s">
@@ -6432,7 +6479,7 @@
         <v>292</v>
       </c>
       <c r="C95" s="27" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D95" s="25"/>
       <c r="E95" s="25" t="s">
@@ -6457,7 +6504,7 @@
         <v>292</v>
       </c>
       <c r="C96" s="27" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D96" s="25"/>
       <c r="E96" s="25" t="s">
@@ -6482,7 +6529,7 @@
         <v>293</v>
       </c>
       <c r="C97" s="27" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D97" s="25"/>
       <c r="E97" s="25" t="s">
@@ -6507,7 +6554,7 @@
         <v>293</v>
       </c>
       <c r="C98" s="27" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D98" s="25"/>
       <c r="E98" s="25" t="s">
@@ -6532,7 +6579,7 @@
         <v>293</v>
       </c>
       <c r="C99" s="27" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D99" s="25"/>
       <c r="E99" s="25" t="s">
@@ -6557,7 +6604,7 @@
         <v>294</v>
       </c>
       <c r="C100" s="27" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D100" s="25"/>
       <c r="E100" s="25" t="s">
@@ -6582,7 +6629,7 @@
         <v>294</v>
       </c>
       <c r="C101" s="27" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D101" s="25"/>
       <c r="E101" s="25" t="s">
@@ -6607,7 +6654,7 @@
         <v>294</v>
       </c>
       <c r="C102" s="27" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="D102" s="25"/>
       <c r="E102" s="25" t="s">
@@ -6632,7 +6679,7 @@
         <v>294</v>
       </c>
       <c r="C103" s="27" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D103" s="25"/>
       <c r="E103" s="25" t="s">
@@ -6657,7 +6704,7 @@
         <v>294</v>
       </c>
       <c r="C104" s="27" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="D104" s="25"/>
       <c r="E104" s="25" t="s">
@@ -6682,7 +6729,7 @@
         <v>295</v>
       </c>
       <c r="C105" s="27" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D105" s="25"/>
       <c r="E105" s="25" t="s">
@@ -6707,7 +6754,7 @@
         <v>295</v>
       </c>
       <c r="C106" s="16" t="s">
-        <v>548</v>
+        <v>537</v>
       </c>
       <c r="D106" s="25"/>
       <c r="E106" s="25" t="s">
@@ -6732,7 +6779,7 @@
         <v>295</v>
       </c>
       <c r="C107" s="27" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D107" s="25"/>
       <c r="E107" s="25" t="s">
@@ -6757,7 +6804,7 @@
         <v>295</v>
       </c>
       <c r="C108" s="27" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D108" s="25"/>
       <c r="E108" s="25" t="s">
@@ -6782,7 +6829,7 @@
         <v>295</v>
       </c>
       <c r="C109" s="16" t="s">
-        <v>563</v>
+        <v>548</v>
       </c>
       <c r="D109" s="25"/>
       <c r="E109" s="25" t="s">
@@ -6807,7 +6854,7 @@
         <v>295</v>
       </c>
       <c r="C110" s="27" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="D110" s="25"/>
       <c r="E110" s="25" t="s">
@@ -6832,7 +6879,7 @@
         <v>295</v>
       </c>
       <c r="C111" s="27" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D111" s="25"/>
       <c r="E111" s="25" t="s">
@@ -6857,7 +6904,7 @@
         <v>295</v>
       </c>
       <c r="C112" s="27" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D112" s="25"/>
       <c r="E112" s="25" t="s">
@@ -6882,7 +6929,7 @@
         <v>295</v>
       </c>
       <c r="C113" s="27" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D113" s="25"/>
       <c r="E113" s="25" t="s">
@@ -6907,7 +6954,7 @@
         <v>295</v>
       </c>
       <c r="C114" s="27" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D114" s="25"/>
       <c r="E114" s="25" t="s">
@@ -6932,7 +6979,7 @@
         <v>296</v>
       </c>
       <c r="C115" s="27" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="D115" s="25"/>
       <c r="E115" s="25" t="s">
@@ -6957,7 +7004,7 @@
         <v>296</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>549</v>
+        <v>538</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="25" t="s">
@@ -6982,7 +7029,7 @@
         <v>296</v>
       </c>
       <c r="C117" s="27" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="25" t="s">
@@ -7007,7 +7054,7 @@
         <v>297</v>
       </c>
       <c r="C118" s="27" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="25" t="s">
@@ -7032,7 +7079,7 @@
         <v>297</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="D119" s="25"/>
       <c r="E119" s="25" t="s">
@@ -7057,7 +7104,7 @@
         <v>297</v>
       </c>
       <c r="C120" s="27" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D120" s="25"/>
       <c r="E120" s="25" t="s">
@@ -7082,7 +7129,7 @@
         <v>297</v>
       </c>
       <c r="C121" s="27" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="25" t="s">
@@ -7107,7 +7154,7 @@
         <v>297</v>
       </c>
       <c r="C122" s="27" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D122" s="25"/>
       <c r="E122" s="25" t="s">
@@ -7132,7 +7179,7 @@
         <v>297</v>
       </c>
       <c r="C123" s="27" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D123" s="25"/>
       <c r="E123" s="25" t="s">
@@ -7157,7 +7204,7 @@
         <v>297</v>
       </c>
       <c r="C124" s="27" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D124" s="25"/>
       <c r="E124" s="25" t="s">
@@ -7182,7 +7229,7 @@
         <v>298</v>
       </c>
       <c r="C125" s="27" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D125" s="25"/>
       <c r="E125" s="25" t="s">
@@ -7207,7 +7254,7 @@
         <v>298</v>
       </c>
       <c r="C126" s="27" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="D126" s="25"/>
       <c r="E126" s="25" t="s">
@@ -7232,7 +7279,7 @@
         <v>298</v>
       </c>
       <c r="C127" s="16" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="D127" s="25"/>
       <c r="E127" s="25" t="s">
@@ -7257,7 +7304,7 @@
         <v>298</v>
       </c>
       <c r="C128" s="27" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D128" s="25"/>
       <c r="E128" s="25" t="s">
@@ -7282,7 +7329,7 @@
         <v>298</v>
       </c>
       <c r="C129" s="27" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="25" t="s">
@@ -7307,7 +7354,7 @@
         <v>298</v>
       </c>
       <c r="C130" s="27" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="D130" s="25"/>
       <c r="E130" s="25" t="s">
@@ -7332,7 +7379,7 @@
         <v>32</v>
       </c>
       <c r="C131" s="27" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D131" s="25"/>
       <c r="E131" s="25" t="s">
@@ -7357,7 +7404,7 @@
         <v>32</v>
       </c>
       <c r="C132" s="27" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="D132" s="25"/>
       <c r="E132" s="25" t="s">
@@ -7382,7 +7429,7 @@
         <v>32</v>
       </c>
       <c r="C133" s="27" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D133" s="25"/>
       <c r="E133" s="25" t="s">
@@ -7407,7 +7454,7 @@
         <v>299</v>
       </c>
       <c r="C134" s="27" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D134" s="25"/>
       <c r="E134" s="25" t="s">
@@ -7432,7 +7479,7 @@
         <v>299</v>
       </c>
       <c r="C135" s="27" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D135" s="25"/>
       <c r="E135" s="25" t="s">
@@ -7457,7 +7504,7 @@
         <v>299</v>
       </c>
       <c r="C136" s="27" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D136" s="25"/>
       <c r="E136" s="25" t="s">
@@ -7482,7 +7529,7 @@
         <v>300</v>
       </c>
       <c r="C137" s="27" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D137" s="25"/>
       <c r="E137" s="25" t="s">
@@ -7507,7 +7554,7 @@
         <v>300</v>
       </c>
       <c r="C138" s="27" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D138" s="25"/>
       <c r="E138" s="25" t="s">
@@ -7532,7 +7579,7 @@
         <v>300</v>
       </c>
       <c r="C139" s="27" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D139" s="25"/>
       <c r="E139" s="25" t="s">
@@ -7557,7 +7604,7 @@
         <v>300</v>
       </c>
       <c r="C140" s="27" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D140" s="25"/>
       <c r="E140" s="25" t="s">
@@ -7582,7 +7629,7 @@
         <v>300</v>
       </c>
       <c r="C141" s="27" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D141" s="25"/>
       <c r="E141" s="25" t="s">
@@ -7607,7 +7654,7 @@
         <v>300</v>
       </c>
       <c r="C142" s="27" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D142" s="25"/>
       <c r="E142" s="25" t="s">
@@ -7632,7 +7679,7 @@
         <v>300</v>
       </c>
       <c r="C143" s="16" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="D143" s="25"/>
       <c r="E143" s="25" t="s">
@@ -7657,7 +7704,7 @@
         <v>300</v>
       </c>
       <c r="C144" s="27" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D144" s="25"/>
       <c r="E144" s="25" t="s">
@@ -7682,7 +7729,7 @@
         <v>300</v>
       </c>
       <c r="C145" s="27" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="25" t="s">
@@ -7707,7 +7754,7 @@
         <v>300</v>
       </c>
       <c r="C146" s="16" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D146" s="25"/>
       <c r="E146" s="25" t="s">
@@ -7732,7 +7779,7 @@
         <v>300</v>
       </c>
       <c r="C147" s="27" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D147" s="25"/>
       <c r="E147" s="25" t="s">
@@ -7757,7 +7804,7 @@
         <v>300</v>
       </c>
       <c r="C148" s="27" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D148" s="25"/>
       <c r="E148" s="25" t="s">
@@ -7782,7 +7829,7 @@
         <v>300</v>
       </c>
       <c r="C149" s="27" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="25" t="s">
@@ -7807,7 +7854,7 @@
         <v>300</v>
       </c>
       <c r="C150" s="16" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="D150" s="25"/>
       <c r="E150" s="25" t="s">
@@ -7832,7 +7879,7 @@
         <v>300</v>
       </c>
       <c r="C151" s="27" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D151" s="25"/>
       <c r="E151" s="25" t="s">
@@ -7857,7 +7904,7 @@
         <v>301</v>
       </c>
       <c r="C152" s="27" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D152" s="25"/>
       <c r="E152" s="25" t="s">
@@ -7882,7 +7929,7 @@
         <v>301</v>
       </c>
       <c r="C153" s="27" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D153" s="25"/>
       <c r="E153" s="25" t="s">
@@ -7907,7 +7954,7 @@
         <v>301</v>
       </c>
       <c r="C154" s="27" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D154" s="25"/>
       <c r="E154" s="25" t="s">
@@ -7932,7 +7979,7 @@
         <v>301</v>
       </c>
       <c r="C155" s="27" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="D155" s="25"/>
       <c r="E155" s="25" t="s">
@@ -7957,7 +8004,7 @@
         <v>301</v>
       </c>
       <c r="C156" s="27" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D156" s="25"/>
       <c r="E156" s="25" t="s">
@@ -7982,7 +8029,7 @@
         <v>301</v>
       </c>
       <c r="C157" s="16" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="D157" s="25"/>
       <c r="E157" s="25" t="s">
@@ -8007,7 +8054,7 @@
         <v>301</v>
       </c>
       <c r="C158" s="27" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D158" s="25"/>
       <c r="E158" s="25" t="s">
@@ -8032,7 +8079,7 @@
         <v>301</v>
       </c>
       <c r="C159" s="27" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D159" s="25"/>
       <c r="E159" s="25" t="s">
@@ -8057,7 +8104,7 @@
         <v>301</v>
       </c>
       <c r="C160" s="27" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D160" s="25"/>
       <c r="E160" s="25" t="s">
@@ -8082,7 +8129,7 @@
         <v>301</v>
       </c>
       <c r="C161" s="27" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D161" s="25"/>
       <c r="E161" s="25" t="s">
@@ -8107,7 +8154,7 @@
         <v>301</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>565</v>
+        <v>550</v>
       </c>
       <c r="D162" s="25"/>
       <c r="E162" s="25" t="s">
@@ -8132,7 +8179,7 @@
         <v>302</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D163" s="25"/>
       <c r="E163" s="25" t="s">
@@ -8157,7 +8204,7 @@
         <v>302</v>
       </c>
       <c r="C164" s="27" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D164" s="25"/>
       <c r="E164" s="25" t="s">
@@ -8182,7 +8229,7 @@
         <v>302</v>
       </c>
       <c r="C165" s="27" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D165" s="25"/>
       <c r="E165" s="25" t="s">
@@ -8207,7 +8254,7 @@
         <v>302</v>
       </c>
       <c r="C166" s="27" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D166" s="25"/>
       <c r="E166" s="25" t="s">
@@ -8232,7 +8279,7 @@
         <v>302</v>
       </c>
       <c r="C167" s="27" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="D167" s="25"/>
       <c r="E167" s="25" t="s">
@@ -8257,7 +8304,7 @@
         <v>303</v>
       </c>
       <c r="C168" s="27" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D168" s="25"/>
       <c r="E168" s="25" t="s">
@@ -8282,7 +8329,7 @@
         <v>303</v>
       </c>
       <c r="C169" s="27" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="D169" s="25"/>
       <c r="E169" s="25" t="s">
@@ -8307,7 +8354,7 @@
         <v>303</v>
       </c>
       <c r="C170" s="27" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D170" s="25"/>
       <c r="E170" s="25" t="s">
@@ -8332,7 +8379,7 @@
         <v>304</v>
       </c>
       <c r="C171" s="27" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="D171" s="25"/>
       <c r="E171" s="25" t="s">
@@ -8357,7 +8404,7 @@
         <v>304</v>
       </c>
       <c r="C172" s="27" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D172" s="25"/>
       <c r="E172" s="25" t="s">
@@ -8382,7 +8429,7 @@
         <v>304</v>
       </c>
       <c r="C173" s="27" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="D173" s="25"/>
       <c r="E173" s="25" t="s">
@@ -8407,7 +8454,7 @@
         <v>305</v>
       </c>
       <c r="C174" s="27" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="D174" s="25"/>
       <c r="E174" s="25" t="s">
@@ -8432,7 +8479,7 @@
         <v>305</v>
       </c>
       <c r="C175" s="27" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D175" s="25"/>
       <c r="E175" s="25" t="s">
@@ -8457,7 +8504,7 @@
         <v>305</v>
       </c>
       <c r="C176" s="27" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="D176" s="25"/>
       <c r="E176" s="25" t="s">
@@ -8482,7 +8529,7 @@
         <v>305</v>
       </c>
       <c r="C177" s="27" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="D177" s="25"/>
       <c r="E177" s="25" t="s">
@@ -8507,7 +8554,7 @@
         <v>305</v>
       </c>
       <c r="C178" s="27" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D178" s="25"/>
       <c r="E178" s="25" t="s">
@@ -8532,7 +8579,7 @@
         <v>305</v>
       </c>
       <c r="C179" s="27" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D179" s="25"/>
       <c r="E179" s="25" t="s">
@@ -8557,7 +8604,7 @@
         <v>306</v>
       </c>
       <c r="C180" s="27" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D180" s="25"/>
       <c r="E180" s="25" t="s">
@@ -8582,7 +8629,7 @@
         <v>306</v>
       </c>
       <c r="C181" s="27" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D181" s="25"/>
       <c r="E181" s="25" t="s">
@@ -8607,7 +8654,7 @@
         <v>306</v>
       </c>
       <c r="C182" s="27" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D182" s="25"/>
       <c r="E182" s="25" t="s">
@@ -8632,7 +8679,7 @@
         <v>306</v>
       </c>
       <c r="C183" s="27" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D183" s="25"/>
       <c r="E183" s="25" t="s">
@@ -8657,7 +8704,7 @@
         <v>306</v>
       </c>
       <c r="C184" s="27" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D184" s="25"/>
       <c r="E184" s="25" t="s">
@@ -8682,7 +8729,7 @@
         <v>307</v>
       </c>
       <c r="C185" s="27" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D185" s="25"/>
       <c r="E185" s="25" t="s">
@@ -8707,7 +8754,7 @@
         <v>307</v>
       </c>
       <c r="C186" s="16" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="D186" s="25"/>
       <c r="E186" s="25" t="s">
@@ -8732,7 +8779,7 @@
         <v>307</v>
       </c>
       <c r="C187" s="27" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D187" s="25"/>
       <c r="E187" s="25" t="s">
@@ -8757,7 +8804,7 @@
         <v>307</v>
       </c>
       <c r="C188" s="27" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D188" s="25"/>
       <c r="E188" s="25" t="s">
@@ -8782,7 +8829,7 @@
         <v>307</v>
       </c>
       <c r="C189" s="16" t="s">
-        <v>564</v>
+        <v>549</v>
       </c>
       <c r="D189" s="25"/>
       <c r="E189" s="25" t="s">
@@ -8807,7 +8854,7 @@
         <v>307</v>
       </c>
       <c r="C190" s="27" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D190" s="25"/>
       <c r="E190" s="25" t="s">
@@ -8832,7 +8879,7 @@
         <v>307</v>
       </c>
       <c r="C191" s="27" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="D191" s="25"/>
       <c r="E191" s="25" t="s">
@@ -8857,7 +8904,7 @@
         <v>308</v>
       </c>
       <c r="C192" s="27" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D192" s="25"/>
       <c r="E192" s="25" t="s">
@@ -8882,7 +8929,7 @@
         <v>308</v>
       </c>
       <c r="C193" s="16" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="D193" s="25"/>
       <c r="E193" s="25" t="s">
@@ -8907,7 +8954,7 @@
         <v>308</v>
       </c>
       <c r="C194" s="27" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D194" s="25"/>
       <c r="E194" s="25" t="s">
@@ -8932,7 +8979,7 @@
         <v>309</v>
       </c>
       <c r="C195" s="27" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D195" s="25"/>
       <c r="E195" s="25" t="s">
@@ -8957,7 +9004,7 @@
         <v>309</v>
       </c>
       <c r="C196" s="16" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="D196" s="25"/>
       <c r="E196" s="25" t="s">
@@ -8982,7 +9029,7 @@
         <v>309</v>
       </c>
       <c r="C197" s="27" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="D197" s="25"/>
       <c r="E197" s="25" t="s">
@@ -9007,7 +9054,7 @@
         <v>309</v>
       </c>
       <c r="C198" s="27" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="D198" s="25"/>
       <c r="E198" s="25" t="s">
@@ -9032,7 +9079,7 @@
         <v>309</v>
       </c>
       <c r="C199" s="27" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="D199" s="25"/>
       <c r="E199" s="25" t="s">
@@ -9057,7 +9104,7 @@
         <v>309</v>
       </c>
       <c r="C200" s="27" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="D200" s="25"/>
       <c r="E200" s="25" t="s">
@@ -9082,7 +9129,7 @@
         <v>309</v>
       </c>
       <c r="C201" s="27" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D201" s="25"/>
       <c r="E201" s="25" t="s">
@@ -9107,7 +9154,7 @@
         <v>310</v>
       </c>
       <c r="C202" s="27" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D202" s="25"/>
       <c r="E202" s="25" t="s">
@@ -9132,7 +9179,7 @@
         <v>310</v>
       </c>
       <c r="C203" s="27" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D203" s="25"/>
       <c r="E203" s="25" t="s">
@@ -9157,7 +9204,7 @@
         <v>310</v>
       </c>
       <c r="C204" s="16" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="D204" s="25"/>
       <c r="E204" s="25" t="s">
@@ -9182,7 +9229,7 @@
         <v>310</v>
       </c>
       <c r="C205" s="27" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D205" s="25"/>
       <c r="E205" s="25" t="s">
@@ -9207,7 +9254,7 @@
         <v>310</v>
       </c>
       <c r="C206" s="27" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="D206" s="25"/>
       <c r="E206" s="25" t="s">
@@ -9232,7 +9279,7 @@
         <v>310</v>
       </c>
       <c r="C207" s="16" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="D207" s="25"/>
       <c r="E207" s="25" t="s">
@@ -9257,7 +9304,7 @@
         <v>310</v>
       </c>
       <c r="C208" s="27" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D208" s="25"/>
       <c r="E208" s="25" t="s">
@@ -9282,7 +9329,7 @@
         <v>310</v>
       </c>
       <c r="C209" s="27" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D209" s="25"/>
       <c r="E209" s="25" t="s">
@@ -9307,7 +9354,7 @@
         <v>310</v>
       </c>
       <c r="C210" s="27" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="D210" s="25"/>
       <c r="E210" s="25" t="s">
@@ -9332,7 +9379,7 @@
         <v>310</v>
       </c>
       <c r="C211" s="27" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D211" s="25"/>
       <c r="E211" s="25" t="s">
@@ -9357,7 +9404,7 @@
         <v>310</v>
       </c>
       <c r="C212" s="27" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D212" s="25"/>
       <c r="E212" s="25" t="s">
@@ -9382,7 +9429,7 @@
         <v>310</v>
       </c>
       <c r="C213" s="27" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D213" s="25"/>
       <c r="E213" s="25" t="s">
@@ -9407,7 +9454,7 @@
         <v>310</v>
       </c>
       <c r="C214" s="27" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D214" s="25"/>
       <c r="E214" s="25" t="s">
@@ -9432,7 +9479,7 @@
         <v>310</v>
       </c>
       <c r="C215" s="27" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="D215" s="25"/>
       <c r="E215" s="25" t="s">
@@ -9457,7 +9504,7 @@
         <v>310</v>
       </c>
       <c r="C216" s="27" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D216" s="25"/>
       <c r="E216" s="25" t="s">
@@ -9482,7 +9529,7 @@
         <v>310</v>
       </c>
       <c r="C217" s="27" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="D217" s="25"/>
       <c r="E217" s="25" t="s">
@@ -9507,7 +9554,7 @@
         <v>310</v>
       </c>
       <c r="C218" s="27" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D218" s="25"/>
       <c r="E218" s="25" t="s">
@@ -9532,7 +9579,7 @@
         <v>310</v>
       </c>
       <c r="C219" s="27" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D219" s="25"/>
       <c r="E219" s="25" t="s">
@@ -9557,7 +9604,7 @@
         <v>311</v>
       </c>
       <c r="C220" s="27" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="D220" s="25"/>
       <c r="E220" s="25" t="s">
@@ -9582,7 +9629,7 @@
         <v>311</v>
       </c>
       <c r="C221" s="27" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="D221" s="25"/>
       <c r="E221" s="25" t="s">
@@ -9607,7 +9654,7 @@
         <v>312</v>
       </c>
       <c r="C222" s="27" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D222" s="25"/>
       <c r="E222" s="25" t="s">
@@ -9632,7 +9679,7 @@
         <v>312</v>
       </c>
       <c r="C223" s="27" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D223" s="25"/>
       <c r="E223" s="25" t="s">
@@ -9657,7 +9704,7 @@
         <v>312</v>
       </c>
       <c r="C224" s="27" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D224" s="25"/>
       <c r="E224" s="25" t="s">
@@ -9682,7 +9729,7 @@
         <v>312</v>
       </c>
       <c r="C225" s="27" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D225" s="25"/>
       <c r="E225" s="25" t="s">
@@ -9707,7 +9754,7 @@
         <v>312</v>
       </c>
       <c r="C226" s="27" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="D226" s="25"/>
       <c r="E226" s="25" t="s">
@@ -9732,7 +9779,7 @@
         <v>312</v>
       </c>
       <c r="C227" s="27" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="D227" s="25"/>
       <c r="E227" s="25" t="s">
@@ -9757,7 +9804,7 @@
         <v>312</v>
       </c>
       <c r="C228" s="27" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="D228" s="25"/>
       <c r="E228" s="25" t="s">
@@ -9782,7 +9829,7 @@
         <v>312</v>
       </c>
       <c r="C229" s="27" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D229" s="25"/>
       <c r="E229" s="25" t="s">
@@ -9807,7 +9854,7 @@
         <v>312</v>
       </c>
       <c r="C230" s="27" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="D230" s="25"/>
       <c r="E230" s="25" t="s">
@@ -9832,7 +9879,7 @@
         <v>312</v>
       </c>
       <c r="C231" s="27" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="D231" s="25"/>
       <c r="E231" s="25" t="s">
@@ -9857,7 +9904,7 @@
         <v>312</v>
       </c>
       <c r="C232" s="27" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="D232" s="25"/>
       <c r="E232" s="25" t="s">
@@ -9882,7 +9929,7 @@
         <v>312</v>
       </c>
       <c r="C233" s="27" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D233" s="25"/>
       <c r="E233" s="25" t="s">
@@ -9907,7 +9954,7 @@
         <v>312</v>
       </c>
       <c r="C234" s="27" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D234" s="25"/>
       <c r="E234" s="25" t="s">
@@ -9932,7 +9979,7 @@
         <v>312</v>
       </c>
       <c r="C235" s="27" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="D235" s="25"/>
       <c r="E235" s="25" t="s">
@@ -9957,7 +10004,7 @@
         <v>312</v>
       </c>
       <c r="C236" s="27" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D236" s="25"/>
       <c r="E236" s="25" t="s">
@@ -9981,8 +10028,8 @@
       <c r="B237" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="C237" s="27" t="s">
-        <v>513</v>
+      <c r="C237" s="16" t="s">
+        <v>558</v>
       </c>
       <c r="D237" s="25"/>
       <c r="E237" s="25" t="s">
@@ -10006,8 +10053,8 @@
       <c r="B238" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="C238" s="27" t="s">
-        <v>514</v>
+      <c r="C238" s="16" t="s">
+        <v>559</v>
       </c>
       <c r="D238" s="25"/>
       <c r="E238" s="25" t="s">
@@ -10032,10 +10079,10 @@
         <v>313</v>
       </c>
       <c r="C239" s="27" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="D239" s="25" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="E239" s="25" t="s">
         <v>22</v>
@@ -10050,7 +10097,7 @@
         <v>21</v>
       </c>
       <c r="I239" s="27" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
     </row>
     <row r="240" spans="1:9" ht="255">
@@ -10060,11 +10107,11 @@
       <c r="B240" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="C240" s="27" t="s">
-        <v>516</v>
+      <c r="C240" s="16" t="s">
+        <v>509</v>
       </c>
       <c r="D240" s="25" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="E240" s="25" t="s">
         <v>22</v>
@@ -10079,7 +10126,7 @@
         <v>20</v>
       </c>
       <c r="I240" s="27" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
     </row>
     <row r="241" spans="1:9" ht="285">
@@ -10090,10 +10137,10 @@
         <v>313</v>
       </c>
       <c r="C241" s="27" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="D241" s="25" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="E241" s="25" t="s">
         <v>22</v>
@@ -10117,10 +10164,10 @@
         <v>313</v>
       </c>
       <c r="C242" s="27" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="D242" s="25" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="E242" s="25" t="s">
         <v>22</v>
@@ -10144,10 +10191,10 @@
         <v>313</v>
       </c>
       <c r="C243" s="27" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="D243" s="25" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="E243" s="25" t="s">
         <v>22</v>
@@ -10164,14 +10211,14 @@
       <c r="I243" s="27"/>
     </row>
     <row r="244" spans="1:9" ht="120">
-      <c r="A244" s="25" t="s">
+      <c r="A244" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="B244" s="26" t="s">
-        <v>314</v>
-      </c>
-      <c r="C244" s="27" t="s">
-        <v>520</v>
+      <c r="B244" s="20" t="s">
+        <v>560</v>
+      </c>
+      <c r="C244" s="16" t="s">
+        <v>513</v>
       </c>
       <c r="D244" s="25"/>
       <c r="E244" s="25" t="s">
@@ -10189,14 +10236,14 @@
       <c r="I244" s="27"/>
     </row>
     <row r="245" spans="1:9" ht="409.5">
-      <c r="A245" s="25" t="s">
+      <c r="A245" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="B245" s="26" t="s">
-        <v>315</v>
+      <c r="B245" s="20" t="s">
+        <v>561</v>
       </c>
       <c r="C245" s="28" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="D245" s="25"/>
       <c r="E245" s="25" t="s">
@@ -10217,11 +10264,11 @@
       <c r="A246" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="B246" s="26" t="s">
-        <v>316</v>
+      <c r="B246" s="20" t="s">
+        <v>562</v>
       </c>
       <c r="C246" s="28" t="s">
-        <v>536</v>
+        <v>563</v>
       </c>
       <c r="D246" s="25"/>
       <c r="E246" s="25" t="s">
@@ -10242,11 +10289,11 @@
       <c r="A247" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="B247" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="C247" s="27" t="s">
-        <v>521</v>
+      <c r="B247" s="20" t="s">
+        <v>564</v>
+      </c>
+      <c r="C247" s="16" t="s">
+        <v>514</v>
       </c>
       <c r="D247" s="25"/>
       <c r="E247" s="25" t="s">
@@ -10268,10 +10315,10 @@
         <v>267</v>
       </c>
       <c r="B248" s="26" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C248" s="27" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="D248" s="25"/>
       <c r="E248" s="25" t="s">
@@ -10292,11 +10339,11 @@
       <c r="A249" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="B249" s="26" t="s">
-        <v>317</v>
+      <c r="B249" s="20" t="s">
+        <v>564</v>
       </c>
       <c r="C249" s="27" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="D249" s="25"/>
       <c r="E249" s="25" t="s">
@@ -10317,11 +10364,11 @@
       <c r="A250" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="B250" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="C250" s="27" t="s">
-        <v>524</v>
+      <c r="B250" s="20" t="s">
+        <v>565</v>
+      </c>
+      <c r="C250" s="16" t="s">
+        <v>517</v>
       </c>
       <c r="D250" s="25"/>
       <c r="E250" s="25" t="s">
@@ -10342,11 +10389,11 @@
       <c r="A251" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="B251" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="C251" s="27" t="s">
-        <v>525</v>
+      <c r="B251" s="20" t="s">
+        <v>565</v>
+      </c>
+      <c r="C251" s="16" t="s">
+        <v>518</v>
       </c>
       <c r="D251" s="25"/>
       <c r="E251" s="25" t="s">
@@ -10367,11 +10414,11 @@
       <c r="A252" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="B252" s="26" t="s">
-        <v>318</v>
+      <c r="B252" s="20" t="s">
+        <v>565</v>
       </c>
       <c r="C252" s="27" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="D252" s="25"/>
       <c r="E252" s="25" t="s">
@@ -10392,11 +10439,11 @@
       <c r="A253" s="25" t="s">
         <v>272</v>
       </c>
-      <c r="B253" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="C253" s="27" t="s">
-        <v>527</v>
+      <c r="B253" s="20" t="s">
+        <v>566</v>
+      </c>
+      <c r="C253" s="16" t="s">
+        <v>520</v>
       </c>
       <c r="D253" s="25"/>
       <c r="E253" s="25" t="s">
@@ -10511,20 +10558,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F253">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F253" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E253">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E253" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G253">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G253" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H253">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H253" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10534,7 +10581,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B244:B255 B10:B16 B18:B243 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B248 B10:B16 B18:B243 B254:B255" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>